<commit_message>
Fixed DPYD phenotype not being dependend on genotype. Fixed ABCB1 genotype: Has to be C-T and not G-A
</commit_message>
<xml_diff>
--- a/Output/Dataframes/complete.xlsx
+++ b/Output/Dataframes/complete.xlsx
@@ -11168,7 +11168,7 @@
         <v>46</v>
       </c>
       <c r="D603" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E603" t="s">
         <v>113</v>
@@ -12154,7 +12154,7 @@
         <v>46</v>
       </c>
       <c r="D661" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E661" t="s">
         <v>113</v>
@@ -19056,7 +19056,7 @@
         <v>46</v>
       </c>
       <c r="D1067" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E1067" t="s">
         <v>113</v>

</xml_diff>

<commit_message>
Fixed CYP2C19 and MTHFR1298 positioning
</commit_message>
<xml_diff>
--- a/Output/Dataframes/complete.xlsx
+++ b/Output/Dataframes/complete.xlsx
@@ -130,13 +130,13 @@
     <t>CYP2B6</t>
   </si>
   <si>
-    <t>CYP2C19</t>
-  </si>
-  <si>
     <t>CYP2C8</t>
   </si>
   <si>
     <t>CYP2C9</t>
+  </si>
+  <si>
+    <t>CYP2C19</t>
   </si>
   <si>
     <t>CYP2D6</t>
@@ -202,10 +202,10 @@
     <t>MC4R</t>
   </si>
   <si>
-    <t>MTHFR1298</t>
+    <t>MTHFR677</t>
   </si>
   <si>
-    <t>MTHFR677</t>
+    <t>MTHFR1298</t>
   </si>
   <si>
     <t>MTNR1B</t>
@@ -316,7 +316,7 @@
     <t>UM</t>
   </si>
   <si>
-    <t>A/A</t>
+    <t>T/T</t>
   </si>
   <si>
     <t>C/G</t>
@@ -340,10 +340,10 @@
     <t>*1/*1</t>
   </si>
   <si>
-    <t>*2/*17</t>
+    <t>*1A/*1C</t>
   </si>
   <si>
-    <t>*1A/*1C</t>
+    <t>*2/*17</t>
   </si>
   <si>
     <t>*2/*4</t>
@@ -356,6 +356,9 @@
   </si>
   <si>
     <t>AS: 2</t>
+  </si>
+  <si>
+    <t>A/A</t>
   </si>
   <si>
     <t>B/B</t>
@@ -371,9 +374,6 @@
   </si>
   <si>
     <t>A/G</t>
-  </si>
-  <si>
-    <t>T/T</t>
   </si>
   <si>
     <t>Null/m.=</t>
@@ -1172,7 +1172,7 @@
         <v>38</v>
       </c>
       <c r="D15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E15" t="s">
         <v>108</v>
@@ -1192,7 +1192,7 @@
         <v>86</v>
       </c>
       <c r="E16" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1206,10 +1206,10 @@
         <v>40</v>
       </c>
       <c r="D17" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E17" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1379,7 +1379,7 @@
         <v>84</v>
       </c>
       <c r="E27" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1396,7 +1396,7 @@
         <v>86</v>
       </c>
       <c r="E28" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1413,7 +1413,7 @@
         <v>84</v>
       </c>
       <c r="E29" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1447,7 +1447,7 @@
         <v>87</v>
       </c>
       <c r="E31" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1481,7 +1481,7 @@
         <v>87</v>
       </c>
       <c r="E33" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1532,7 +1532,7 @@
         <v>84</v>
       </c>
       <c r="E36" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1566,7 +1566,7 @@
         <v>84</v>
       </c>
       <c r="E38" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1580,7 +1580,7 @@
         <v>62</v>
       </c>
       <c r="D39" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E39" t="s">
         <v>100</v>
@@ -1597,10 +1597,10 @@
         <v>63</v>
       </c>
       <c r="D40" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E40" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1651,7 +1651,7 @@
         <v>84</v>
       </c>
       <c r="E43" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1719,7 +1719,7 @@
         <v>86</v>
       </c>
       <c r="E47" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1821,7 +1821,7 @@
         <v>84</v>
       </c>
       <c r="E53" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1872,7 +1872,7 @@
         <v>84</v>
       </c>
       <c r="E56" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -1906,7 +1906,7 @@
         <v>84</v>
       </c>
       <c r="E58" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -1991,7 +1991,7 @@
         <v>84</v>
       </c>
       <c r="E63" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -2161,7 +2161,7 @@
         <v>87</v>
       </c>
       <c r="E73" t="s">
-        <v>108</v>
+        <v>129</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -2175,10 +2175,10 @@
         <v>39</v>
       </c>
       <c r="D74" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E74" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -2192,10 +2192,10 @@
         <v>40</v>
       </c>
       <c r="D75" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E75" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -2365,7 +2365,7 @@
         <v>84</v>
       </c>
       <c r="E85" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="86" spans="1:5">
@@ -2399,7 +2399,7 @@
         <v>84</v>
       </c>
       <c r="E87" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -2467,7 +2467,7 @@
         <v>87</v>
       </c>
       <c r="E91" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="92" spans="1:5">
@@ -2518,7 +2518,7 @@
         <v>84</v>
       </c>
       <c r="E94" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -2552,7 +2552,7 @@
         <v>84</v>
       </c>
       <c r="E96" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="97" spans="1:5">
@@ -2569,7 +2569,7 @@
         <v>87</v>
       </c>
       <c r="E97" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
     </row>
     <row r="98" spans="1:5">
@@ -2586,7 +2586,7 @@
         <v>87</v>
       </c>
       <c r="E98" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
     </row>
     <row r="99" spans="1:5">
@@ -2637,7 +2637,7 @@
         <v>84</v>
       </c>
       <c r="E101" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="102" spans="1:5">
@@ -2688,7 +2688,7 @@
         <v>84</v>
       </c>
       <c r="E104" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="105" spans="1:5">
@@ -2705,7 +2705,7 @@
         <v>86</v>
       </c>
       <c r="E105" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -2807,7 +2807,7 @@
         <v>84</v>
       </c>
       <c r="E111" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="112" spans="1:5">
@@ -2824,7 +2824,7 @@
         <v>84</v>
       </c>
       <c r="E112" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="113" spans="1:5">
@@ -2858,7 +2858,7 @@
         <v>84</v>
       </c>
       <c r="E114" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="115" spans="1:5">
@@ -2892,7 +2892,7 @@
         <v>84</v>
       </c>
       <c r="E116" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="117" spans="1:5">
@@ -2926,7 +2926,7 @@
         <v>87</v>
       </c>
       <c r="E118" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
     </row>
     <row r="119" spans="1:5">
@@ -3011,7 +3011,7 @@
         <v>84</v>
       </c>
       <c r="E123" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="124" spans="1:5">
@@ -3028,7 +3028,7 @@
         <v>84</v>
       </c>
       <c r="E124" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="125" spans="1:5">
@@ -3147,7 +3147,7 @@
         <v>86</v>
       </c>
       <c r="E131" t="s">
-        <v>107</v>
+        <v>139</v>
       </c>
     </row>
     <row r="132" spans="1:5">
@@ -3164,7 +3164,7 @@
         <v>86</v>
       </c>
       <c r="E132" t="s">
-        <v>139</v>
+        <v>107</v>
       </c>
     </row>
     <row r="133" spans="1:5">
@@ -3368,7 +3368,7 @@
         <v>86</v>
       </c>
       <c r="E144" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="145" spans="1:5">
@@ -3385,7 +3385,7 @@
         <v>84</v>
       </c>
       <c r="E145" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="146" spans="1:5">
@@ -3453,7 +3453,7 @@
         <v>87</v>
       </c>
       <c r="E149" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="150" spans="1:5">
@@ -3487,7 +3487,7 @@
         <v>84</v>
       </c>
       <c r="E151" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="152" spans="1:5">
@@ -3504,7 +3504,7 @@
         <v>84</v>
       </c>
       <c r="E152" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="153" spans="1:5">
@@ -3552,7 +3552,7 @@
         <v>62</v>
       </c>
       <c r="D155" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E155" t="s">
         <v>100</v>
@@ -3569,10 +3569,10 @@
         <v>63</v>
       </c>
       <c r="D156" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E156" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="157" spans="1:5">
@@ -3623,7 +3623,7 @@
         <v>84</v>
       </c>
       <c r="E159" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="160" spans="1:5">
@@ -3691,7 +3691,7 @@
         <v>86</v>
       </c>
       <c r="E163" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="164" spans="1:5">
@@ -3793,7 +3793,7 @@
         <v>84</v>
       </c>
       <c r="E169" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="170" spans="1:5">
@@ -3810,7 +3810,7 @@
         <v>84</v>
       </c>
       <c r="E170" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="171" spans="1:5">
@@ -3878,7 +3878,7 @@
         <v>84</v>
       </c>
       <c r="E174" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="175" spans="1:5">
@@ -3912,7 +3912,7 @@
         <v>87</v>
       </c>
       <c r="E176" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
     </row>
     <row r="177" spans="1:5">
@@ -4130,7 +4130,7 @@
         <v>38</v>
       </c>
       <c r="D189" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E189" t="s">
         <v>108</v>
@@ -4150,7 +4150,7 @@
         <v>86</v>
       </c>
       <c r="E190" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="191" spans="1:5">
@@ -4164,10 +4164,10 @@
         <v>40</v>
       </c>
       <c r="D191" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E191" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="192" spans="1:5">
@@ -4337,7 +4337,7 @@
         <v>84</v>
       </c>
       <c r="E201" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="202" spans="1:5">
@@ -4354,7 +4354,7 @@
         <v>86</v>
       </c>
       <c r="E202" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="203" spans="1:5">
@@ -4371,7 +4371,7 @@
         <v>84</v>
       </c>
       <c r="E203" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="204" spans="1:5">
@@ -4439,7 +4439,7 @@
         <v>87</v>
       </c>
       <c r="E207" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="208" spans="1:5">
@@ -4456,7 +4456,7 @@
         <v>84</v>
       </c>
       <c r="E208" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="209" spans="1:5">
@@ -4473,7 +4473,7 @@
         <v>84</v>
       </c>
       <c r="E209" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="210" spans="1:5">
@@ -4524,7 +4524,7 @@
         <v>84</v>
       </c>
       <c r="E212" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="213" spans="1:5">
@@ -4541,7 +4541,7 @@
         <v>87</v>
       </c>
       <c r="E213" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
     </row>
     <row r="214" spans="1:5">
@@ -4558,7 +4558,7 @@
         <v>87</v>
       </c>
       <c r="E214" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
     </row>
     <row r="215" spans="1:5">
@@ -4609,7 +4609,7 @@
         <v>84</v>
       </c>
       <c r="E217" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="218" spans="1:5">
@@ -4677,7 +4677,7 @@
         <v>86</v>
       </c>
       <c r="E221" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="222" spans="1:5">
@@ -4779,7 +4779,7 @@
         <v>84</v>
       </c>
       <c r="E227" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="228" spans="1:5">
@@ -4830,7 +4830,7 @@
         <v>84</v>
       </c>
       <c r="E230" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="231" spans="1:5">
@@ -4864,7 +4864,7 @@
         <v>84</v>
       </c>
       <c r="E232" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="233" spans="1:5">
@@ -4898,7 +4898,7 @@
         <v>87</v>
       </c>
       <c r="E234" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
     </row>
     <row r="235" spans="1:5">
@@ -4949,7 +4949,7 @@
         <v>84</v>
       </c>
       <c r="E237" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="238" spans="1:5">
@@ -5119,7 +5119,7 @@
         <v>86</v>
       </c>
       <c r="E247" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="248" spans="1:5">
@@ -5136,7 +5136,7 @@
         <v>86</v>
       </c>
       <c r="E248" t="s">
-        <v>139</v>
+        <v>107</v>
       </c>
     </row>
     <row r="249" spans="1:5">
@@ -5153,7 +5153,7 @@
         <v>86</v>
       </c>
       <c r="E249" t="s">
-        <v>107</v>
+        <v>147</v>
       </c>
     </row>
     <row r="250" spans="1:5">
@@ -5357,7 +5357,7 @@
         <v>84</v>
       </c>
       <c r="E261" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="262" spans="1:5">
@@ -5374,7 +5374,7 @@
         <v>84</v>
       </c>
       <c r="E262" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="263" spans="1:5">
@@ -5442,7 +5442,7 @@
         <v>84</v>
       </c>
       <c r="E266" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="267" spans="1:5">
@@ -5476,7 +5476,7 @@
         <v>84</v>
       </c>
       <c r="E268" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="269" spans="1:5">
@@ -5524,7 +5524,7 @@
         <v>62</v>
       </c>
       <c r="D271" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E271" t="s">
         <v>103</v>
@@ -5541,7 +5541,7 @@
         <v>63</v>
       </c>
       <c r="D272" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E272" t="s">
         <v>103</v>
@@ -5595,7 +5595,7 @@
         <v>84</v>
       </c>
       <c r="E275" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="276" spans="1:5">
@@ -5663,7 +5663,7 @@
         <v>86</v>
       </c>
       <c r="E279" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="280" spans="1:5">
@@ -5748,7 +5748,7 @@
         <v>84</v>
       </c>
       <c r="E284" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="285" spans="1:5">
@@ -5765,7 +5765,7 @@
         <v>84</v>
       </c>
       <c r="E285" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="286" spans="1:5">
@@ -5816,7 +5816,7 @@
         <v>84</v>
       </c>
       <c r="E288" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="289" spans="1:5">
@@ -5850,7 +5850,7 @@
         <v>84</v>
       </c>
       <c r="E290" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="291" spans="1:5">
@@ -6105,7 +6105,7 @@
         <v>86</v>
       </c>
       <c r="E305" t="s">
-        <v>107</v>
+        <v>139</v>
       </c>
     </row>
     <row r="306" spans="1:5">
@@ -6119,10 +6119,10 @@
         <v>39</v>
       </c>
       <c r="D306" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E306" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
     </row>
     <row r="307" spans="1:5">
@@ -6136,10 +6136,10 @@
         <v>40</v>
       </c>
       <c r="D307" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E307" t="s">
-        <v>153</v>
+        <v>107</v>
       </c>
     </row>
     <row r="308" spans="1:5">
@@ -6309,7 +6309,7 @@
         <v>84</v>
       </c>
       <c r="E317" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="318" spans="1:5">
@@ -6326,7 +6326,7 @@
         <v>86</v>
       </c>
       <c r="E318" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="319" spans="1:5">
@@ -6343,7 +6343,7 @@
         <v>84</v>
       </c>
       <c r="E319" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="320" spans="1:5">
@@ -6462,7 +6462,7 @@
         <v>84</v>
       </c>
       <c r="E326" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="327" spans="1:5">
@@ -6510,10 +6510,10 @@
         <v>62</v>
       </c>
       <c r="D329" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E329" t="s">
-        <v>135</v>
+        <v>103</v>
       </c>
     </row>
     <row r="330" spans="1:5">
@@ -6527,10 +6527,10 @@
         <v>63</v>
       </c>
       <c r="D330" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E330" t="s">
-        <v>103</v>
+        <v>135</v>
       </c>
     </row>
     <row r="331" spans="1:5">
@@ -6581,7 +6581,7 @@
         <v>84</v>
       </c>
       <c r="E333" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="334" spans="1:5">
@@ -6649,7 +6649,7 @@
         <v>86</v>
       </c>
       <c r="E337" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="338" spans="1:5">
@@ -6751,7 +6751,7 @@
         <v>84</v>
       </c>
       <c r="E343" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="344" spans="1:5">
@@ -6802,7 +6802,7 @@
         <v>84</v>
       </c>
       <c r="E346" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="347" spans="1:5">
@@ -6836,7 +6836,7 @@
         <v>84</v>
       </c>
       <c r="E348" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="349" spans="1:5">
@@ -6870,7 +6870,7 @@
         <v>86</v>
       </c>
       <c r="E350" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="351" spans="1:5">
@@ -7088,10 +7088,10 @@
         <v>38</v>
       </c>
       <c r="D363" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E363" t="s">
-        <v>108</v>
+        <v>157</v>
       </c>
     </row>
     <row r="364" spans="1:5">
@@ -7108,7 +7108,7 @@
         <v>86</v>
       </c>
       <c r="E364" t="s">
-        <v>157</v>
+        <v>107</v>
       </c>
     </row>
     <row r="365" spans="1:5">
@@ -7122,10 +7122,10 @@
         <v>40</v>
       </c>
       <c r="D365" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E365" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="366" spans="1:5">
@@ -7312,7 +7312,7 @@
         <v>86</v>
       </c>
       <c r="E376" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="377" spans="1:5">
@@ -7329,7 +7329,7 @@
         <v>84</v>
       </c>
       <c r="E377" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="378" spans="1:5">
@@ -7346,7 +7346,7 @@
         <v>84</v>
       </c>
       <c r="E378" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="379" spans="1:5">
@@ -7397,7 +7397,7 @@
         <v>87</v>
       </c>
       <c r="E381" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="382" spans="1:5">
@@ -7448,7 +7448,7 @@
         <v>84</v>
       </c>
       <c r="E384" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="385" spans="1:5">
@@ -7482,7 +7482,7 @@
         <v>84</v>
       </c>
       <c r="E386" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="387" spans="1:5">
@@ -7499,7 +7499,7 @@
         <v>86</v>
       </c>
       <c r="E387" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="388" spans="1:5">
@@ -7516,7 +7516,7 @@
         <v>86</v>
       </c>
       <c r="E388" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
     </row>
     <row r="389" spans="1:5">
@@ -7567,7 +7567,7 @@
         <v>84</v>
       </c>
       <c r="E391" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="392" spans="1:5">
@@ -7635,7 +7635,7 @@
         <v>86</v>
       </c>
       <c r="E395" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="396" spans="1:5">
@@ -7737,7 +7737,7 @@
         <v>84</v>
       </c>
       <c r="E401" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="402" spans="1:5">
@@ -7754,7 +7754,7 @@
         <v>84</v>
       </c>
       <c r="E402" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="403" spans="1:5">
@@ -7788,7 +7788,7 @@
         <v>84</v>
       </c>
       <c r="E404" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="405" spans="1:5">
@@ -7822,7 +7822,7 @@
         <v>84</v>
       </c>
       <c r="E406" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="407" spans="1:5">
@@ -7856,7 +7856,7 @@
         <v>87</v>
       </c>
       <c r="E408" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
     </row>
     <row r="409" spans="1:5">
@@ -8074,10 +8074,10 @@
         <v>38</v>
       </c>
       <c r="D421" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E421" t="s">
-        <v>108</v>
+        <v>157</v>
       </c>
     </row>
     <row r="422" spans="1:5">
@@ -8094,7 +8094,7 @@
         <v>86</v>
       </c>
       <c r="E422" t="s">
-        <v>157</v>
+        <v>107</v>
       </c>
     </row>
     <row r="423" spans="1:5">
@@ -8108,10 +8108,10 @@
         <v>40</v>
       </c>
       <c r="D423" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E423" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="424" spans="1:5">
@@ -8315,7 +8315,7 @@
         <v>84</v>
       </c>
       <c r="E435" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="436" spans="1:5">
@@ -8383,7 +8383,7 @@
         <v>87</v>
       </c>
       <c r="E439" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="440" spans="1:5">
@@ -8400,7 +8400,7 @@
         <v>84</v>
       </c>
       <c r="E440" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="441" spans="1:5">
@@ -8434,7 +8434,7 @@
         <v>84</v>
       </c>
       <c r="E442" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="443" spans="1:5">
@@ -8468,7 +8468,7 @@
         <v>84</v>
       </c>
       <c r="E444" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="445" spans="1:5">
@@ -8485,7 +8485,7 @@
         <v>87</v>
       </c>
       <c r="E445" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
     </row>
     <row r="446" spans="1:5">
@@ -8502,7 +8502,7 @@
         <v>87</v>
       </c>
       <c r="E446" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
     </row>
     <row r="447" spans="1:5">
@@ -8553,7 +8553,7 @@
         <v>84</v>
       </c>
       <c r="E449" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="450" spans="1:5">
@@ -8621,7 +8621,7 @@
         <v>86</v>
       </c>
       <c r="E453" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="454" spans="1:5">
@@ -8723,7 +8723,7 @@
         <v>84</v>
       </c>
       <c r="E459" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="460" spans="1:5">
@@ -8808,7 +8808,7 @@
         <v>84</v>
       </c>
       <c r="E464" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="465" spans="1:5">
@@ -9060,10 +9060,10 @@
         <v>38</v>
       </c>
       <c r="D479" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E479" t="s">
-        <v>108</v>
+        <v>139</v>
       </c>
     </row>
     <row r="480" spans="1:5">
@@ -9080,7 +9080,7 @@
         <v>86</v>
       </c>
       <c r="E480" t="s">
-        <v>139</v>
+        <v>107</v>
       </c>
     </row>
     <row r="481" spans="1:5">
@@ -9094,10 +9094,10 @@
         <v>40</v>
       </c>
       <c r="D481" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E481" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="482" spans="1:5">
@@ -9267,7 +9267,7 @@
         <v>84</v>
       </c>
       <c r="E491" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="492" spans="1:5">
@@ -9284,7 +9284,7 @@
         <v>86</v>
       </c>
       <c r="E492" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="493" spans="1:5">
@@ -9301,7 +9301,7 @@
         <v>84</v>
       </c>
       <c r="E493" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="494" spans="1:5">
@@ -9318,7 +9318,7 @@
         <v>84</v>
       </c>
       <c r="E494" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="495" spans="1:5">
@@ -9369,7 +9369,7 @@
         <v>87</v>
       </c>
       <c r="E497" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="498" spans="1:5">
@@ -9420,7 +9420,7 @@
         <v>84</v>
       </c>
       <c r="E500" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="501" spans="1:5">
@@ -9454,7 +9454,7 @@
         <v>84</v>
       </c>
       <c r="E502" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="503" spans="1:5">
@@ -9468,10 +9468,10 @@
         <v>62</v>
       </c>
       <c r="D503" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E503" t="s">
-        <v>100</v>
+        <v>123</v>
       </c>
     </row>
     <row r="504" spans="1:5">
@@ -9485,10 +9485,10 @@
         <v>63</v>
       </c>
       <c r="D504" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E504" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="505" spans="1:5">
@@ -9539,7 +9539,7 @@
         <v>84</v>
       </c>
       <c r="E507" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="508" spans="1:5">
@@ -9607,7 +9607,7 @@
         <v>86</v>
       </c>
       <c r="E511" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="512" spans="1:5">
@@ -9709,7 +9709,7 @@
         <v>84</v>
       </c>
       <c r="E517" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="518" spans="1:5">
@@ -9726,7 +9726,7 @@
         <v>84</v>
       </c>
       <c r="E518" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="519" spans="1:5">
@@ -9760,7 +9760,7 @@
         <v>84</v>
       </c>
       <c r="E520" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="521" spans="1:5">
@@ -9794,7 +9794,7 @@
         <v>84</v>
       </c>
       <c r="E522" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="523" spans="1:5">
@@ -9828,7 +9828,7 @@
         <v>87</v>
       </c>
       <c r="E524" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
     </row>
     <row r="525" spans="1:5">
@@ -9879,7 +9879,7 @@
         <v>84</v>
       </c>
       <c r="E527" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="528" spans="1:5">
@@ -10046,10 +10046,10 @@
         <v>38</v>
       </c>
       <c r="D537" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E537" t="s">
-        <v>108</v>
+        <v>139</v>
       </c>
     </row>
     <row r="538" spans="1:5">
@@ -10066,7 +10066,7 @@
         <v>86</v>
       </c>
       <c r="E538" t="s">
-        <v>139</v>
+        <v>107</v>
       </c>
     </row>
     <row r="539" spans="1:5">
@@ -10080,10 +10080,10 @@
         <v>40</v>
       </c>
       <c r="D539" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E539" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="540" spans="1:5">
@@ -10253,7 +10253,7 @@
         <v>84</v>
       </c>
       <c r="E549" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="550" spans="1:5">
@@ -10287,7 +10287,7 @@
         <v>84</v>
       </c>
       <c r="E551" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="552" spans="1:5">
@@ -10355,7 +10355,7 @@
         <v>87</v>
       </c>
       <c r="E555" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="556" spans="1:5">
@@ -10372,7 +10372,7 @@
         <v>84</v>
       </c>
       <c r="E556" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="557" spans="1:5">
@@ -10389,7 +10389,7 @@
         <v>84</v>
       </c>
       <c r="E557" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="558" spans="1:5">
@@ -10440,7 +10440,7 @@
         <v>84</v>
       </c>
       <c r="E560" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="561" spans="1:5">
@@ -10454,10 +10454,10 @@
         <v>62</v>
       </c>
       <c r="D561" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E561" t="s">
-        <v>100</v>
+        <v>123</v>
       </c>
     </row>
     <row r="562" spans="1:5">
@@ -10471,10 +10471,10 @@
         <v>63</v>
       </c>
       <c r="D562" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E562" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="563" spans="1:5">
@@ -10525,7 +10525,7 @@
         <v>84</v>
       </c>
       <c r="E565" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="566" spans="1:5">
@@ -10593,7 +10593,7 @@
         <v>86</v>
       </c>
       <c r="E569" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="570" spans="1:5">
@@ -10695,7 +10695,7 @@
         <v>84</v>
       </c>
       <c r="E575" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="576" spans="1:5">
@@ -10746,7 +10746,7 @@
         <v>84</v>
       </c>
       <c r="E578" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="579" spans="1:5">
@@ -10780,7 +10780,7 @@
         <v>84</v>
       </c>
       <c r="E580" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="581" spans="1:5">
@@ -10814,7 +10814,7 @@
         <v>87</v>
       </c>
       <c r="E582" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
     </row>
     <row r="583" spans="1:5">
@@ -10865,7 +10865,7 @@
         <v>84</v>
       </c>
       <c r="E585" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="586" spans="1:5">
@@ -11035,7 +11035,7 @@
         <v>86</v>
       </c>
       <c r="E595" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="596" spans="1:5">
@@ -11052,7 +11052,7 @@
         <v>86</v>
       </c>
       <c r="E596" t="s">
-        <v>139</v>
+        <v>107</v>
       </c>
     </row>
     <row r="597" spans="1:5">
@@ -11069,7 +11069,7 @@
         <v>86</v>
       </c>
       <c r="E597" t="s">
-        <v>107</v>
+        <v>147</v>
       </c>
     </row>
     <row r="598" spans="1:5">
@@ -11239,7 +11239,7 @@
         <v>84</v>
       </c>
       <c r="E607" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="608" spans="1:5">
@@ -11273,7 +11273,7 @@
         <v>84</v>
       </c>
       <c r="E609" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="610" spans="1:5">
@@ -11392,7 +11392,7 @@
         <v>84</v>
       </c>
       <c r="E616" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="617" spans="1:5">
@@ -11443,7 +11443,7 @@
         <v>87</v>
       </c>
       <c r="E619" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
     </row>
     <row r="620" spans="1:5">
@@ -11460,7 +11460,7 @@
         <v>87</v>
       </c>
       <c r="E620" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
     </row>
     <row r="621" spans="1:5">
@@ -11511,7 +11511,7 @@
         <v>84</v>
       </c>
       <c r="E623" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="624" spans="1:5">
@@ -11562,7 +11562,7 @@
         <v>84</v>
       </c>
       <c r="E626" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="627" spans="1:5">
@@ -11579,7 +11579,7 @@
         <v>86</v>
       </c>
       <c r="E627" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="628" spans="1:5">
@@ -11681,7 +11681,7 @@
         <v>84</v>
       </c>
       <c r="E633" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="634" spans="1:5">
@@ -11766,7 +11766,7 @@
         <v>84</v>
       </c>
       <c r="E638" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="639" spans="1:5">
@@ -11800,7 +11800,7 @@
         <v>87</v>
       </c>
       <c r="E640" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
     </row>
     <row r="641" spans="1:5">
@@ -11851,7 +11851,7 @@
         <v>84</v>
       </c>
       <c r="E643" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="644" spans="1:5">
@@ -12021,7 +12021,7 @@
         <v>86</v>
       </c>
       <c r="E653" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="654" spans="1:5">
@@ -12038,7 +12038,7 @@
         <v>86</v>
       </c>
       <c r="E654" t="s">
-        <v>139</v>
+        <v>107</v>
       </c>
     </row>
     <row r="655" spans="1:5">
@@ -12055,7 +12055,7 @@
         <v>86</v>
       </c>
       <c r="E655" t="s">
-        <v>107</v>
+        <v>147</v>
       </c>
     </row>
     <row r="656" spans="1:5">
@@ -12225,7 +12225,7 @@
         <v>84</v>
       </c>
       <c r="E665" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="666" spans="1:5">
@@ -12259,7 +12259,7 @@
         <v>84</v>
       </c>
       <c r="E667" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="668" spans="1:5">
@@ -12378,7 +12378,7 @@
         <v>84</v>
       </c>
       <c r="E674" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="675" spans="1:5">
@@ -12429,7 +12429,7 @@
         <v>87</v>
       </c>
       <c r="E677" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
     </row>
     <row r="678" spans="1:5">
@@ -12446,7 +12446,7 @@
         <v>87</v>
       </c>
       <c r="E678" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
     </row>
     <row r="679" spans="1:5">
@@ -12497,7 +12497,7 @@
         <v>84</v>
       </c>
       <c r="E681" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="682" spans="1:5">
@@ -12548,7 +12548,7 @@
         <v>84</v>
       </c>
       <c r="E684" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="685" spans="1:5">
@@ -12565,7 +12565,7 @@
         <v>86</v>
       </c>
       <c r="E685" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="686" spans="1:5">
@@ -12667,7 +12667,7 @@
         <v>84</v>
       </c>
       <c r="E691" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="692" spans="1:5">
@@ -12752,7 +12752,7 @@
         <v>84</v>
       </c>
       <c r="E696" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="697" spans="1:5">
@@ -12786,7 +12786,7 @@
         <v>86</v>
       </c>
       <c r="E698" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="699" spans="1:5">
@@ -13007,7 +13007,7 @@
         <v>87</v>
       </c>
       <c r="E711" t="s">
-        <v>108</v>
+        <v>168</v>
       </c>
     </row>
     <row r="712" spans="1:5">
@@ -13024,7 +13024,7 @@
         <v>87</v>
       </c>
       <c r="E712" t="s">
-        <v>168</v>
+        <v>128</v>
       </c>
     </row>
     <row r="713" spans="1:5">
@@ -13041,7 +13041,7 @@
         <v>87</v>
       </c>
       <c r="E713" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
     </row>
     <row r="714" spans="1:5">
@@ -13245,7 +13245,7 @@
         <v>84</v>
       </c>
       <c r="E725" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="726" spans="1:5">
@@ -13412,7 +13412,7 @@
         <v>62</v>
       </c>
       <c r="D735" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E735" t="s">
         <v>100</v>
@@ -13429,10 +13429,10 @@
         <v>63</v>
       </c>
       <c r="D736" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E736" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="737" spans="1:5">
@@ -13483,7 +13483,7 @@
         <v>84</v>
       </c>
       <c r="E739" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="740" spans="1:5">
@@ -13534,7 +13534,7 @@
         <v>84</v>
       </c>
       <c r="E742" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="743" spans="1:5">
@@ -13551,7 +13551,7 @@
         <v>86</v>
       </c>
       <c r="E743" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="744" spans="1:5">
@@ -13704,7 +13704,7 @@
         <v>84</v>
       </c>
       <c r="E752" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="753" spans="1:5">
@@ -13772,7 +13772,7 @@
         <v>87</v>
       </c>
       <c r="E756" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
     </row>
     <row r="757" spans="1:5">
@@ -13823,7 +13823,7 @@
         <v>84</v>
       </c>
       <c r="E759" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="760" spans="1:5">
@@ -13993,7 +13993,7 @@
         <v>86</v>
       </c>
       <c r="E769" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="770" spans="1:5">
@@ -14010,7 +14010,7 @@
         <v>86</v>
       </c>
       <c r="E770" t="s">
-        <v>139</v>
+        <v>107</v>
       </c>
     </row>
     <row r="771" spans="1:5">
@@ -14027,7 +14027,7 @@
         <v>86</v>
       </c>
       <c r="E771" t="s">
-        <v>107</v>
+        <v>147</v>
       </c>
     </row>
     <row r="772" spans="1:5">
@@ -14197,7 +14197,7 @@
         <v>84</v>
       </c>
       <c r="E781" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="782" spans="1:5">
@@ -14214,7 +14214,7 @@
         <v>86</v>
       </c>
       <c r="E782" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="783" spans="1:5">
@@ -14231,7 +14231,7 @@
         <v>84</v>
       </c>
       <c r="E783" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="784" spans="1:5">
@@ -14248,7 +14248,7 @@
         <v>84</v>
       </c>
       <c r="E784" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="785" spans="1:5">
@@ -14299,7 +14299,7 @@
         <v>87</v>
       </c>
       <c r="E787" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="788" spans="1:5">
@@ -14316,7 +14316,7 @@
         <v>84</v>
       </c>
       <c r="E788" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="789" spans="1:5">
@@ -14333,7 +14333,7 @@
         <v>84</v>
       </c>
       <c r="E789" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="790" spans="1:5">
@@ -14350,7 +14350,7 @@
         <v>84</v>
       </c>
       <c r="E790" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="791" spans="1:5">
@@ -14384,7 +14384,7 @@
         <v>84</v>
       </c>
       <c r="E792" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="793" spans="1:5">
@@ -14398,10 +14398,10 @@
         <v>62</v>
       </c>
       <c r="D793" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E793" t="s">
-        <v>100</v>
+        <v>123</v>
       </c>
     </row>
     <row r="794" spans="1:5">
@@ -14415,10 +14415,10 @@
         <v>63</v>
       </c>
       <c r="D794" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E794" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="795" spans="1:5">
@@ -14469,7 +14469,7 @@
         <v>84</v>
       </c>
       <c r="E797" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="798" spans="1:5">
@@ -14537,7 +14537,7 @@
         <v>86</v>
       </c>
       <c r="E801" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="802" spans="1:5">
@@ -14588,7 +14588,7 @@
         <v>84</v>
       </c>
       <c r="E804" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="805" spans="1:5">
@@ -14639,7 +14639,7 @@
         <v>84</v>
       </c>
       <c r="E807" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="808" spans="1:5">
@@ -14724,7 +14724,7 @@
         <v>84</v>
       </c>
       <c r="E812" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="813" spans="1:5">
@@ -14758,7 +14758,7 @@
         <v>86</v>
       </c>
       <c r="E814" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="815" spans="1:5">
@@ -14979,7 +14979,7 @@
         <v>86</v>
       </c>
       <c r="E827" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="828" spans="1:5">
@@ -14996,7 +14996,7 @@
         <v>86</v>
       </c>
       <c r="E828" t="s">
-        <v>139</v>
+        <v>107</v>
       </c>
     </row>
     <row r="829" spans="1:5">
@@ -15013,7 +15013,7 @@
         <v>86</v>
       </c>
       <c r="E829" t="s">
-        <v>107</v>
+        <v>147</v>
       </c>
     </row>
     <row r="830" spans="1:5">
@@ -15183,7 +15183,7 @@
         <v>84</v>
       </c>
       <c r="E839" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="840" spans="1:5">
@@ -15200,7 +15200,7 @@
         <v>86</v>
       </c>
       <c r="E840" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="841" spans="1:5">
@@ -15217,7 +15217,7 @@
         <v>84</v>
       </c>
       <c r="E841" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="842" spans="1:5">
@@ -15234,7 +15234,7 @@
         <v>84</v>
       </c>
       <c r="E842" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="843" spans="1:5">
@@ -15285,7 +15285,7 @@
         <v>87</v>
       </c>
       <c r="E845" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="846" spans="1:5">
@@ -15370,7 +15370,7 @@
         <v>84</v>
       </c>
       <c r="E850" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="851" spans="1:5">
@@ -15384,10 +15384,10 @@
         <v>62</v>
       </c>
       <c r="D851" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E851" t="s">
-        <v>135</v>
+        <v>103</v>
       </c>
     </row>
     <row r="852" spans="1:5">
@@ -15401,10 +15401,10 @@
         <v>63</v>
       </c>
       <c r="D852" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E852" t="s">
-        <v>103</v>
+        <v>135</v>
       </c>
     </row>
     <row r="853" spans="1:5">
@@ -15455,7 +15455,7 @@
         <v>84</v>
       </c>
       <c r="E855" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="856" spans="1:5">
@@ -15506,7 +15506,7 @@
         <v>84</v>
       </c>
       <c r="E858" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="859" spans="1:5">
@@ -15523,7 +15523,7 @@
         <v>86</v>
       </c>
       <c r="E859" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="860" spans="1:5">
@@ -15625,7 +15625,7 @@
         <v>84</v>
       </c>
       <c r="E865" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="866" spans="1:5">
@@ -15676,7 +15676,7 @@
         <v>84</v>
       </c>
       <c r="E868" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="869" spans="1:5">
@@ -15710,7 +15710,7 @@
         <v>84</v>
       </c>
       <c r="E870" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="871" spans="1:5">
@@ -15795,7 +15795,7 @@
         <v>84</v>
       </c>
       <c r="E875" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="876" spans="1:5">
@@ -15965,7 +15965,7 @@
         <v>86</v>
       </c>
       <c r="E885" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
     <row r="886" spans="1:5">
@@ -15982,7 +15982,7 @@
         <v>86</v>
       </c>
       <c r="E886" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="887" spans="1:5">
@@ -16169,7 +16169,7 @@
         <v>84</v>
       </c>
       <c r="E897" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="898" spans="1:5">
@@ -16203,7 +16203,7 @@
         <v>84</v>
       </c>
       <c r="E899" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="900" spans="1:5">
@@ -16271,7 +16271,7 @@
         <v>87</v>
       </c>
       <c r="E903" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="904" spans="1:5">
@@ -16305,7 +16305,7 @@
         <v>84</v>
       </c>
       <c r="E905" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="906" spans="1:5">
@@ -16322,7 +16322,7 @@
         <v>84</v>
       </c>
       <c r="E906" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="907" spans="1:5">
@@ -16370,7 +16370,7 @@
         <v>62</v>
       </c>
       <c r="D909" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E909" t="s">
         <v>100</v>
@@ -16387,10 +16387,10 @@
         <v>63</v>
       </c>
       <c r="D910" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E910" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="911" spans="1:5">
@@ -16441,7 +16441,7 @@
         <v>84</v>
       </c>
       <c r="E913" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="914" spans="1:5">
@@ -16509,7 +16509,7 @@
         <v>86</v>
       </c>
       <c r="E917" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="918" spans="1:5">
@@ -16611,7 +16611,7 @@
         <v>84</v>
       </c>
       <c r="E923" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="924" spans="1:5">
@@ -16662,7 +16662,7 @@
         <v>84</v>
       </c>
       <c r="E926" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="927" spans="1:5">
@@ -16696,7 +16696,7 @@
         <v>84</v>
       </c>
       <c r="E928" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="929" spans="1:5">
@@ -16951,7 +16951,7 @@
         <v>86</v>
       </c>
       <c r="E943" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="944" spans="1:5">
@@ -16968,7 +16968,7 @@
         <v>86</v>
       </c>
       <c r="E944" t="s">
-        <v>139</v>
+        <v>107</v>
       </c>
     </row>
     <row r="945" spans="1:5">
@@ -16985,7 +16985,7 @@
         <v>86</v>
       </c>
       <c r="E945" t="s">
-        <v>107</v>
+        <v>147</v>
       </c>
     </row>
     <row r="946" spans="1:5">
@@ -17155,7 +17155,7 @@
         <v>84</v>
       </c>
       <c r="E955" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="956" spans="1:5">
@@ -17172,7 +17172,7 @@
         <v>86</v>
       </c>
       <c r="E956" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="957" spans="1:5">
@@ -17189,7 +17189,7 @@
         <v>84</v>
       </c>
       <c r="E957" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="958" spans="1:5">
@@ -17223,7 +17223,7 @@
         <v>87</v>
       </c>
       <c r="E959" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="960" spans="1:5">
@@ -17308,7 +17308,7 @@
         <v>84</v>
       </c>
       <c r="E964" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="965" spans="1:5">
@@ -17359,7 +17359,7 @@
         <v>87</v>
       </c>
       <c r="E967" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
     </row>
     <row r="968" spans="1:5">
@@ -17376,7 +17376,7 @@
         <v>87</v>
       </c>
       <c r="E968" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
     </row>
     <row r="969" spans="1:5">
@@ -17495,7 +17495,7 @@
         <v>86</v>
       </c>
       <c r="E975" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="976" spans="1:5">
@@ -17597,7 +17597,7 @@
         <v>84</v>
       </c>
       <c r="E981" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="982" spans="1:5">
@@ -17614,7 +17614,7 @@
         <v>84</v>
       </c>
       <c r="E982" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="983" spans="1:5">
@@ -17648,7 +17648,7 @@
         <v>84</v>
       </c>
       <c r="E984" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="985" spans="1:5">
@@ -17682,7 +17682,7 @@
         <v>84</v>
       </c>
       <c r="E986" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="987" spans="1:5">
@@ -17716,7 +17716,7 @@
         <v>86</v>
       </c>
       <c r="E988" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="989" spans="1:5">
@@ -17934,10 +17934,10 @@
         <v>38</v>
       </c>
       <c r="D1001" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="E1001" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
     </row>
     <row r="1002" spans="1:5">
@@ -17954,7 +17954,7 @@
         <v>86</v>
       </c>
       <c r="E1002" t="s">
-        <v>157</v>
+        <v>107</v>
       </c>
     </row>
     <row r="1003" spans="1:5">
@@ -17968,10 +17968,10 @@
         <v>40</v>
       </c>
       <c r="D1003" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="E1003" t="s">
-        <v>107</v>
+        <v>176</v>
       </c>
     </row>
     <row r="1004" spans="1:5">
@@ -18175,7 +18175,7 @@
         <v>84</v>
       </c>
       <c r="E1015" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="1016" spans="1:5">
@@ -18243,7 +18243,7 @@
         <v>87</v>
       </c>
       <c r="E1019" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="1020" spans="1:5">
@@ -18260,7 +18260,7 @@
         <v>84</v>
       </c>
       <c r="E1020" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="1021" spans="1:5">
@@ -18277,7 +18277,7 @@
         <v>84</v>
       </c>
       <c r="E1021" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="1022" spans="1:5">
@@ -18345,7 +18345,7 @@
         <v>87</v>
       </c>
       <c r="E1025" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
     </row>
     <row r="1026" spans="1:5">
@@ -18362,7 +18362,7 @@
         <v>87</v>
       </c>
       <c r="E1026" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
     </row>
     <row r="1027" spans="1:5">
@@ -18413,7 +18413,7 @@
         <v>84</v>
       </c>
       <c r="E1029" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="1030" spans="1:5">
@@ -18481,7 +18481,7 @@
         <v>86</v>
       </c>
       <c r="E1033" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="1034" spans="1:5">
@@ -18583,7 +18583,7 @@
         <v>84</v>
       </c>
       <c r="E1039" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="1040" spans="1:5">
@@ -18600,7 +18600,7 @@
         <v>84</v>
       </c>
       <c r="E1040" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="1041" spans="1:5">
@@ -18634,7 +18634,7 @@
         <v>84</v>
       </c>
       <c r="E1042" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="1043" spans="1:5">
@@ -18668,7 +18668,7 @@
         <v>84</v>
       </c>
       <c r="E1044" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="1045" spans="1:5">
@@ -18702,7 +18702,7 @@
         <v>87</v>
       </c>
       <c r="E1046" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
     </row>
     <row r="1047" spans="1:5">
@@ -18753,7 +18753,7 @@
         <v>84</v>
       </c>
       <c r="E1049" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="1050" spans="1:5">
@@ -18920,7 +18920,7 @@
         <v>38</v>
       </c>
       <c r="D1059" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E1059" t="s">
         <v>108</v>
@@ -18940,7 +18940,7 @@
         <v>86</v>
       </c>
       <c r="E1060" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="1061" spans="1:5">
@@ -18954,10 +18954,10 @@
         <v>40</v>
       </c>
       <c r="D1061" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E1061" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="1062" spans="1:5">
@@ -19127,7 +19127,7 @@
         <v>84</v>
       </c>
       <c r="E1071" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="1072" spans="1:5">
@@ -19144,7 +19144,7 @@
         <v>86</v>
       </c>
       <c r="E1072" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="1073" spans="1:5">
@@ -19161,7 +19161,7 @@
         <v>84</v>
       </c>
       <c r="E1073" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="1074" spans="1:5">
@@ -19178,7 +19178,7 @@
         <v>84</v>
       </c>
       <c r="E1074" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="1075" spans="1:5">
@@ -19229,7 +19229,7 @@
         <v>87</v>
       </c>
       <c r="E1077" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="1078" spans="1:5">
@@ -19331,7 +19331,7 @@
         <v>86</v>
       </c>
       <c r="E1083" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="1084" spans="1:5">
@@ -19348,7 +19348,7 @@
         <v>86</v>
       </c>
       <c r="E1084" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
     </row>
     <row r="1085" spans="1:5">
@@ -19399,7 +19399,7 @@
         <v>84</v>
       </c>
       <c r="E1087" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="1088" spans="1:5">
@@ -19450,7 +19450,7 @@
         <v>84</v>
       </c>
       <c r="E1090" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="1091" spans="1:5">
@@ -19467,7 +19467,7 @@
         <v>87</v>
       </c>
       <c r="E1091" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="1092" spans="1:5">
@@ -19569,7 +19569,7 @@
         <v>84</v>
       </c>
       <c r="E1097" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="1098" spans="1:5">
@@ -19620,7 +19620,7 @@
         <v>84</v>
       </c>
       <c r="E1100" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="1101" spans="1:5">
@@ -19654,7 +19654,7 @@
         <v>84</v>
       </c>
       <c r="E1102" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="1103" spans="1:5">
@@ -19688,7 +19688,7 @@
         <v>87</v>
       </c>
       <c r="E1104" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
     </row>
     <row r="1105" spans="1:5">
@@ -19909,7 +19909,7 @@
         <v>86</v>
       </c>
       <c r="E1117" t="s">
-        <v>107</v>
+        <v>179</v>
       </c>
     </row>
     <row r="1118" spans="1:5">
@@ -19926,7 +19926,7 @@
         <v>86</v>
       </c>
       <c r="E1118" t="s">
-        <v>179</v>
+        <v>107</v>
       </c>
     </row>
     <row r="1119" spans="1:5">
@@ -20113,7 +20113,7 @@
         <v>84</v>
       </c>
       <c r="E1129" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="1130" spans="1:5">
@@ -20147,7 +20147,7 @@
         <v>84</v>
       </c>
       <c r="E1131" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="1132" spans="1:5">
@@ -20215,7 +20215,7 @@
         <v>87</v>
       </c>
       <c r="E1135" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="1136" spans="1:5">
@@ -20266,7 +20266,7 @@
         <v>84</v>
       </c>
       <c r="E1138" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="1139" spans="1:5">
@@ -20317,7 +20317,7 @@
         <v>87</v>
       </c>
       <c r="E1141" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
     </row>
     <row r="1142" spans="1:5">
@@ -20334,7 +20334,7 @@
         <v>87</v>
       </c>
       <c r="E1142" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
     </row>
     <row r="1143" spans="1:5">
@@ -20385,7 +20385,7 @@
         <v>84</v>
       </c>
       <c r="E1145" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="1146" spans="1:5">
@@ -20453,7 +20453,7 @@
         <v>86</v>
       </c>
       <c r="E1149" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="1150" spans="1:5">
@@ -20504,7 +20504,7 @@
         <v>84</v>
       </c>
       <c r="E1152" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="1153" spans="1:5">
@@ -20555,7 +20555,7 @@
         <v>84</v>
       </c>
       <c r="E1155" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="1156" spans="1:5">
@@ -20606,7 +20606,7 @@
         <v>84</v>
       </c>
       <c r="E1158" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="1159" spans="1:5">
@@ -20674,7 +20674,7 @@
         <v>87</v>
       </c>
       <c r="E1162" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
     </row>
     <row r="1163" spans="1:5">
@@ -20725,7 +20725,7 @@
         <v>84</v>
       </c>
       <c r="E1165" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="1166" spans="1:5">
@@ -20892,10 +20892,10 @@
         <v>38</v>
       </c>
       <c r="D1175" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E1175" t="s">
-        <v>108</v>
+        <v>182</v>
       </c>
     </row>
     <row r="1176" spans="1:5">
@@ -20912,7 +20912,7 @@
         <v>86</v>
       </c>
       <c r="E1176" t="s">
-        <v>182</v>
+        <v>107</v>
       </c>
     </row>
     <row r="1177" spans="1:5">
@@ -20926,10 +20926,10 @@
         <v>40</v>
       </c>
       <c r="D1177" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E1177" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="1178" spans="1:5">
@@ -21065,7 +21065,7 @@
         <v>96</v>
       </c>
       <c r="E1185" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="1186" spans="1:5">
@@ -21099,7 +21099,7 @@
         <v>84</v>
       </c>
       <c r="E1187" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="1188" spans="1:5">
@@ -21116,7 +21116,7 @@
         <v>86</v>
       </c>
       <c r="E1188" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="1189" spans="1:5">
@@ -21133,7 +21133,7 @@
         <v>84</v>
       </c>
       <c r="E1189" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="1190" spans="1:5">
@@ -21150,7 +21150,7 @@
         <v>84</v>
       </c>
       <c r="E1190" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="1191" spans="1:5">
@@ -21167,7 +21167,7 @@
         <v>87</v>
       </c>
       <c r="E1191" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="1192" spans="1:5">
@@ -21218,7 +21218,7 @@
         <v>84</v>
       </c>
       <c r="E1194" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="1195" spans="1:5">
@@ -21252,7 +21252,7 @@
         <v>84</v>
       </c>
       <c r="E1196" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="1197" spans="1:5">
@@ -21269,7 +21269,7 @@
         <v>84</v>
       </c>
       <c r="E1197" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="1198" spans="1:5">
@@ -21297,13 +21297,13 @@
         <v>24</v>
       </c>
       <c r="C1199" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D1199" t="s">
         <v>86</v>
       </c>
       <c r="E1199" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="1200" spans="1:5">
@@ -21314,7 +21314,7 @@
         <v>24</v>
       </c>
       <c r="C1200" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D1200" t="s">
         <v>87</v>
@@ -21371,7 +21371,7 @@
         <v>84</v>
       </c>
       <c r="E1203" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="1204" spans="1:5">
@@ -21439,7 +21439,7 @@
         <v>86</v>
       </c>
       <c r="E1207" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="1208" spans="1:5">
@@ -21490,7 +21490,7 @@
         <v>84</v>
       </c>
       <c r="E1210" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="1211" spans="1:5">
@@ -21507,7 +21507,7 @@
         <v>84</v>
       </c>
       <c r="E1211" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="1212" spans="1:5">
@@ -21524,7 +21524,7 @@
         <v>84</v>
       </c>
       <c r="E1212" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
     </row>
     <row r="1213" spans="1:5">
@@ -21541,7 +21541,7 @@
         <v>84</v>
       </c>
       <c r="E1213" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="1214" spans="1:5">
@@ -21592,7 +21592,7 @@
         <v>84</v>
       </c>
       <c r="E1216" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
     </row>
     <row r="1217" spans="1:5">
@@ -21626,7 +21626,7 @@
         <v>84</v>
       </c>
       <c r="E1218" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="1219" spans="1:5">

</xml_diff>

<commit_message>
Genotype en Fenotype vorm kloppen nu
</commit_message>
<xml_diff>
--- a/Output/Dataframes/complete.xlsx
+++ b/Output/Dataframes/complete.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14998" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14998" uniqueCount="304">
   <si>
     <t>sample_id</t>
   </si>
@@ -643,13 +643,13 @@
     <t>Kalyan-Kerala/Null</t>
   </si>
   <si>
-    <t>present</t>
+    <t>Present</t>
   </si>
   <si>
     <t>*A/*C</t>
   </si>
   <si>
-    <t>c.103T&gt;C/WT</t>
+    <t>MT/WT</t>
   </si>
   <si>
     <t>521TC</t>
@@ -665,9 +665,6 @@
   </si>
   <si>
     <t>*28/*60</t>
-  </si>
-  <si>
-    <t>F508del/WT</t>
   </si>
   <si>
     <t>*8/*9+1F</t>
@@ -704,9 +701,6 @@
   </si>
   <si>
     <t>*2/*4</t>
-  </si>
-  <si>
-    <t>MT/WT</t>
   </si>
   <si>
     <t>*4/*10</t>
@@ -752,9 +746,6 @@
   </si>
   <si>
     <t>521CC</t>
-  </si>
-  <si>
-    <t>R117H/WT</t>
   </si>
   <si>
     <t>*1/*12</t>
@@ -805,7 +796,7 @@
     <t>*B/*C</t>
   </si>
   <si>
-    <t>*1C/1F</t>
+    <t>*1C/*1F</t>
   </si>
   <si>
     <t>*1/*18</t>
@@ -908,9 +899,6 @@
   </si>
   <si>
     <t>*4/*26</t>
-  </si>
-  <si>
-    <t>*1/*2,*2/*3</t>
   </si>
   <si>
     <t>G/A</t>
@@ -7024,7 +7012,7 @@
         <v>139</v>
       </c>
       <c r="E337" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="338" spans="1:5">
@@ -7092,7 +7080,7 @@
         <v>134</v>
       </c>
       <c r="E341" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="342" spans="1:5">
@@ -7211,7 +7199,7 @@
         <v>133</v>
       </c>
       <c r="E348" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="349" spans="1:5">
@@ -7228,7 +7216,7 @@
         <v>133</v>
       </c>
       <c r="E349" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="350" spans="1:5">
@@ -7449,7 +7437,7 @@
         <v>130</v>
       </c>
       <c r="E362" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="363" spans="1:5">
@@ -7466,7 +7454,7 @@
         <v>134</v>
       </c>
       <c r="E363" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="364" spans="1:5">
@@ -7687,7 +7675,7 @@
         <v>144</v>
       </c>
       <c r="E376" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="377" spans="1:5">
@@ -8282,7 +8270,7 @@
         <v>130</v>
       </c>
       <c r="E411" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="412" spans="1:5">
@@ -8316,7 +8304,7 @@
         <v>133</v>
       </c>
       <c r="E413" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="414" spans="1:5">
@@ -8333,7 +8321,7 @@
         <v>133</v>
       </c>
       <c r="E414" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="415" spans="1:5">
@@ -8554,7 +8542,7 @@
         <v>130</v>
       </c>
       <c r="E427" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="428" spans="1:5">
@@ -8792,7 +8780,7 @@
         <v>137</v>
       </c>
       <c r="E441" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="442" spans="1:5">
@@ -9047,7 +9035,7 @@
         <v>130</v>
       </c>
       <c r="E456" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="457" spans="1:5">
@@ -9370,7 +9358,7 @@
         <v>133</v>
       </c>
       <c r="E475" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="476" spans="1:5">
@@ -9421,7 +9409,7 @@
         <v>134</v>
       </c>
       <c r="E478" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="479" spans="1:5">
@@ -9659,7 +9647,7 @@
         <v>130</v>
       </c>
       <c r="E492" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="493" spans="1:5">
@@ -9676,7 +9664,7 @@
         <v>134</v>
       </c>
       <c r="E493" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="494" spans="1:5">
@@ -9999,7 +9987,7 @@
         <v>143</v>
       </c>
       <c r="E512" t="s">
-        <v>230</v>
+        <v>211</v>
       </c>
     </row>
     <row r="513" spans="1:5">
@@ -10526,7 +10514,7 @@
         <v>134</v>
       </c>
       <c r="E543" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="544" spans="1:5">
@@ -10543,7 +10531,7 @@
         <v>133</v>
       </c>
       <c r="E544" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="545" spans="1:5">
@@ -10764,7 +10752,7 @@
         <v>130</v>
       </c>
       <c r="E557" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="558" spans="1:5">
@@ -11002,7 +10990,7 @@
         <v>137</v>
       </c>
       <c r="E571" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="572" spans="1:5">
@@ -11206,7 +11194,7 @@
         <v>134</v>
       </c>
       <c r="E583" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="584" spans="1:5">
@@ -11563,7 +11551,7 @@
         <v>134</v>
       </c>
       <c r="E604" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="605" spans="1:5">
@@ -11869,7 +11857,7 @@
         <v>130</v>
       </c>
       <c r="E622" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="623" spans="1:5">
@@ -11886,7 +11874,7 @@
         <v>134</v>
       </c>
       <c r="E623" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="624" spans="1:5">
@@ -12566,7 +12554,7 @@
         <v>133</v>
       </c>
       <c r="E663" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="664" spans="1:5">
@@ -12668,7 +12656,7 @@
         <v>134</v>
       </c>
       <c r="E669" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="670" spans="1:5">
@@ -12821,7 +12809,7 @@
         <v>147</v>
       </c>
       <c r="E678" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="679" spans="1:5">
@@ -12940,7 +12928,7 @@
         <v>133</v>
       </c>
       <c r="E685" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="686" spans="1:5">
@@ -13076,7 +13064,7 @@
         <v>132</v>
       </c>
       <c r="E693" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="694" spans="1:5">
@@ -13450,7 +13438,7 @@
         <v>133</v>
       </c>
       <c r="E715" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="716" spans="1:5">
@@ -13790,7 +13778,7 @@
         <v>134</v>
       </c>
       <c r="E735" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="736" spans="1:5">
@@ -13841,7 +13829,7 @@
         <v>134</v>
       </c>
       <c r="E738" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="739" spans="1:5">
@@ -14079,7 +14067,7 @@
         <v>130</v>
       </c>
       <c r="E752" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="753" spans="1:5">
@@ -14096,7 +14084,7 @@
         <v>134</v>
       </c>
       <c r="E753" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="754" spans="1:5">
@@ -14181,7 +14169,7 @@
         <v>132</v>
       </c>
       <c r="E758" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="759" spans="1:5">
@@ -14317,7 +14305,7 @@
         <v>137</v>
       </c>
       <c r="E766" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="767" spans="1:5">
@@ -14436,7 +14424,7 @@
         <v>148</v>
       </c>
       <c r="E773" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="774" spans="1:5">
@@ -14878,7 +14866,7 @@
         <v>133</v>
       </c>
       <c r="E799" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="800" spans="1:5">
@@ -15184,7 +15172,7 @@
         <v>130</v>
       </c>
       <c r="E817" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="818" spans="1:5">
@@ -15201,7 +15189,7 @@
         <v>134</v>
       </c>
       <c r="E818" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="819" spans="1:5">
@@ -15864,7 +15852,7 @@
         <v>139</v>
       </c>
       <c r="E857" t="s">
-        <v>246</v>
+        <v>211</v>
       </c>
     </row>
     <row r="858" spans="1:5">
@@ -16000,7 +15988,7 @@
         <v>133</v>
       </c>
       <c r="E865" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="866" spans="1:5">
@@ -16051,7 +16039,7 @@
         <v>133</v>
       </c>
       <c r="E868" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="869" spans="1:5">
@@ -16289,7 +16277,7 @@
         <v>130</v>
       </c>
       <c r="E882" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="883" spans="1:5">
@@ -16986,7 +16974,7 @@
         <v>133</v>
       </c>
       <c r="E923" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="924" spans="1:5">
@@ -17071,7 +17059,7 @@
         <v>134</v>
       </c>
       <c r="E928" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="929" spans="1:5">
@@ -17156,7 +17144,7 @@
         <v>134</v>
       </c>
       <c r="E933" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="934" spans="1:5">
@@ -17173,7 +17161,7 @@
         <v>133</v>
       </c>
       <c r="E934" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="935" spans="1:5">
@@ -17275,7 +17263,7 @@
         <v>134</v>
       </c>
       <c r="E940" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="941" spans="1:5">
@@ -17394,7 +17382,7 @@
         <v>130</v>
       </c>
       <c r="E947" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="948" spans="1:5">
@@ -18091,7 +18079,7 @@
         <v>133</v>
       </c>
       <c r="E988" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="989" spans="1:5">
@@ -18210,7 +18198,7 @@
         <v>134</v>
       </c>
       <c r="E995" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="996" spans="1:5">
@@ -18261,7 +18249,7 @@
         <v>133</v>
       </c>
       <c r="E998" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="999" spans="1:5">
@@ -18278,7 +18266,7 @@
         <v>133</v>
       </c>
       <c r="E999" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="1000" spans="1:5">
@@ -18601,7 +18589,7 @@
         <v>132</v>
       </c>
       <c r="E1018" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="1019" spans="1:5">
@@ -18737,7 +18725,7 @@
         <v>144</v>
       </c>
       <c r="E1026" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="1027" spans="1:5">
@@ -19196,7 +19184,7 @@
         <v>133</v>
       </c>
       <c r="E1053" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="1054" spans="1:5">
@@ -19281,7 +19269,7 @@
         <v>134</v>
       </c>
       <c r="E1058" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="1059" spans="1:5">
@@ -19451,7 +19439,7 @@
         <v>147</v>
       </c>
       <c r="E1068" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="1069" spans="1:5">
@@ -19621,7 +19609,7 @@
         <v>134</v>
       </c>
       <c r="E1078" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="1079" spans="1:5">
@@ -19842,7 +19830,7 @@
         <v>144</v>
       </c>
       <c r="E1091" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="1092" spans="1:5">
@@ -20709,7 +20697,7 @@
         <v>130</v>
       </c>
       <c r="E1142" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="1143" spans="1:5">
@@ -20726,7 +20714,7 @@
         <v>134</v>
       </c>
       <c r="E1143" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="1144" spans="1:5">
@@ -20811,7 +20799,7 @@
         <v>132</v>
       </c>
       <c r="E1148" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="1149" spans="1:5">
@@ -20947,7 +20935,7 @@
         <v>137</v>
       </c>
       <c r="E1156" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="1157" spans="1:5">
@@ -21049,7 +21037,7 @@
         <v>138</v>
       </c>
       <c r="E1162" t="s">
-        <v>230</v>
+        <v>211</v>
       </c>
     </row>
     <row r="1163" spans="1:5">
@@ -21508,7 +21496,7 @@
         <v>133</v>
       </c>
       <c r="E1189" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="1190" spans="1:5">
@@ -21576,7 +21564,7 @@
         <v>134</v>
       </c>
       <c r="E1193" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="1194" spans="1:5">
@@ -22630,7 +22618,7 @@
         <v>134</v>
       </c>
       <c r="E1255" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="1256" spans="1:5">
@@ -22664,7 +22652,7 @@
         <v>130</v>
       </c>
       <c r="E1257" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="1258" spans="1:5">
@@ -22681,7 +22669,7 @@
         <v>133</v>
       </c>
       <c r="E1258" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="1259" spans="1:5">
@@ -23157,7 +23145,7 @@
         <v>144</v>
       </c>
       <c r="E1286" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="1287" spans="1:5">
@@ -23735,7 +23723,7 @@
         <v>141</v>
       </c>
       <c r="E1320" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="1321" spans="1:5">
@@ -23786,7 +23774,7 @@
         <v>133</v>
       </c>
       <c r="E1323" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="1324" spans="1:5">
@@ -24024,7 +24012,7 @@
         <v>130</v>
       </c>
       <c r="E1337" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="1338" spans="1:5">
@@ -24041,7 +24029,7 @@
         <v>134</v>
       </c>
       <c r="E1338" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="1339" spans="1:5">
@@ -24126,7 +24114,7 @@
         <v>132</v>
       </c>
       <c r="E1343" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="1344" spans="1:5">
@@ -24806,7 +24794,7 @@
         <v>134</v>
       </c>
       <c r="E1383" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="1384" spans="1:5">
@@ -24908,7 +24896,7 @@
         <v>133</v>
       </c>
       <c r="E1389" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="1390" spans="1:5">
@@ -25877,7 +25865,7 @@
         <v>134</v>
       </c>
       <c r="E1446" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="1447" spans="1:5">
@@ -25962,7 +25950,7 @@
         <v>134</v>
       </c>
       <c r="E1451" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="1452" spans="1:5">
@@ -26013,7 +26001,7 @@
         <v>133</v>
       </c>
       <c r="E1454" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="1455" spans="1:5">
@@ -26251,7 +26239,7 @@
         <v>134</v>
       </c>
       <c r="E1468" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="1469" spans="1:5">
@@ -26455,7 +26443,7 @@
         <v>137</v>
       </c>
       <c r="E1480" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="1481" spans="1:5">
@@ -26574,7 +26562,7 @@
         <v>143</v>
       </c>
       <c r="E1487" t="s">
-        <v>230</v>
+        <v>211</v>
       </c>
     </row>
     <row r="1488" spans="1:5">
@@ -27033,7 +27021,7 @@
         <v>133</v>
       </c>
       <c r="E1514" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="1515" spans="1:5">
@@ -27101,7 +27089,7 @@
         <v>134</v>
       </c>
       <c r="E1518" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="1519" spans="1:5">
@@ -27356,7 +27344,7 @@
         <v>134</v>
       </c>
       <c r="E1533" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="1534" spans="1:5">
@@ -27679,7 +27667,7 @@
         <v>138</v>
       </c>
       <c r="E1552" t="s">
-        <v>230</v>
+        <v>211</v>
       </c>
     </row>
     <row r="1553" spans="1:5">
@@ -28087,7 +28075,7 @@
         <v>133</v>
       </c>
       <c r="E1576" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="1577" spans="1:5">
@@ -28138,7 +28126,7 @@
         <v>133</v>
       </c>
       <c r="E1579" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="1580" spans="1:5">
@@ -28223,7 +28211,7 @@
         <v>133</v>
       </c>
       <c r="E1584" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="1585" spans="1:5">
@@ -28257,7 +28245,7 @@
         <v>133</v>
       </c>
       <c r="E1586" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="1587" spans="1:5">
@@ -28444,7 +28432,7 @@
         <v>130</v>
       </c>
       <c r="E1597" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="1598" spans="1:5">
@@ -28784,7 +28772,7 @@
         <v>143</v>
       </c>
       <c r="E1617" t="s">
-        <v>230</v>
+        <v>211</v>
       </c>
     </row>
     <row r="1618" spans="1:5">
@@ -29311,7 +29299,7 @@
         <v>133</v>
       </c>
       <c r="E1648" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="1649" spans="1:5">
@@ -29549,7 +29537,7 @@
         <v>130</v>
       </c>
       <c r="E1662" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="1663" spans="1:5">
@@ -29787,7 +29775,7 @@
         <v>144</v>
       </c>
       <c r="E1676" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="1677" spans="1:5">
@@ -30042,7 +30030,7 @@
         <v>130</v>
       </c>
       <c r="E1691" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="1692" spans="1:5">
@@ -30365,7 +30353,7 @@
         <v>133</v>
       </c>
       <c r="E1710" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="1711" spans="1:5">
@@ -30416,7 +30404,7 @@
         <v>134</v>
       </c>
       <c r="E1713" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="1714" spans="1:5">
@@ -30671,7 +30659,7 @@
         <v>134</v>
       </c>
       <c r="E1728" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="1729" spans="1:5">
@@ -31521,7 +31509,7 @@
         <v>134</v>
       </c>
       <c r="E1778" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="1779" spans="1:5">
@@ -31759,7 +31747,7 @@
         <v>130</v>
       </c>
       <c r="E1792" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="1793" spans="1:5">
@@ -31997,7 +31985,7 @@
         <v>144</v>
       </c>
       <c r="E1806" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="1807" spans="1:5">
@@ -32099,7 +32087,7 @@
         <v>138</v>
       </c>
       <c r="E1812" t="s">
-        <v>230</v>
+        <v>211</v>
       </c>
     </row>
     <row r="1813" spans="1:5">
@@ -32558,7 +32546,7 @@
         <v>133</v>
       </c>
       <c r="E1839" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="1840" spans="1:5">
@@ -32864,7 +32852,7 @@
         <v>130</v>
       </c>
       <c r="E1857" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="1858" spans="1:5">
@@ -32966,7 +32954,7 @@
         <v>132</v>
       </c>
       <c r="E1863" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="1864" spans="1:5">
@@ -34309,7 +34297,7 @@
         <v>138</v>
       </c>
       <c r="E1942" t="s">
-        <v>230</v>
+        <v>211</v>
       </c>
     </row>
     <row r="1943" spans="1:5">
@@ -34326,7 +34314,7 @@
         <v>148</v>
       </c>
       <c r="E1943" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="1944" spans="1:5">
@@ -34785,7 +34773,7 @@
         <v>141</v>
       </c>
       <c r="E1970" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="1971" spans="1:5">
@@ -34819,7 +34807,7 @@
         <v>130</v>
       </c>
       <c r="E1972" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="1973" spans="1:5">
@@ -34836,7 +34824,7 @@
         <v>133</v>
       </c>
       <c r="E1973" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="1974" spans="1:5">
@@ -35074,7 +35062,7 @@
         <v>130</v>
       </c>
       <c r="E1987" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="1988" spans="1:5">
@@ -35550,7 +35538,7 @@
         <v>133</v>
       </c>
       <c r="E2015" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="2016" spans="1:5">
@@ -35567,7 +35555,7 @@
         <v>130</v>
       </c>
       <c r="E2016" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2017" spans="1:5">
@@ -35754,7 +35742,7 @@
         <v>139</v>
       </c>
       <c r="E2027" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2028" spans="1:5">
@@ -35822,7 +35810,7 @@
         <v>134</v>
       </c>
       <c r="E2031" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2032" spans="1:5">
@@ -35907,7 +35895,7 @@
         <v>134</v>
       </c>
       <c r="E2036" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="2037" spans="1:5">
@@ -35941,7 +35929,7 @@
         <v>133</v>
       </c>
       <c r="E2038" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="2039" spans="1:5">
@@ -36060,7 +36048,7 @@
         <v>134</v>
       </c>
       <c r="E2045" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="2046" spans="1:5">
@@ -36995,7 +36983,7 @@
         <v>134</v>
       </c>
       <c r="E2100" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2101" spans="1:5">
@@ -37063,7 +37051,7 @@
         <v>133</v>
       </c>
       <c r="E2104" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2105" spans="1:5">
@@ -37284,7 +37272,7 @@
         <v>130</v>
       </c>
       <c r="E2117" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2118" spans="1:5">
@@ -37777,7 +37765,7 @@
         <v>130</v>
       </c>
       <c r="E2146" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2147" spans="1:5">
@@ -37981,7 +37969,7 @@
         <v>133</v>
       </c>
       <c r="E2158" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="2159" spans="1:5">
@@ -38083,7 +38071,7 @@
         <v>133</v>
       </c>
       <c r="E2164" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2165" spans="1:5">
@@ -38151,7 +38139,7 @@
         <v>133</v>
       </c>
       <c r="E2168" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="2169" spans="1:5">
@@ -38627,7 +38615,7 @@
         <v>144</v>
       </c>
       <c r="E2196" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="2197" spans="1:5">
@@ -39137,7 +39125,7 @@
         <v>134</v>
       </c>
       <c r="E2226" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="2227" spans="1:5">
@@ -39222,7 +39210,7 @@
         <v>134</v>
       </c>
       <c r="E2231" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="2232" spans="1:5">
@@ -39256,7 +39244,7 @@
         <v>134</v>
       </c>
       <c r="E2233" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2234" spans="1:5">
@@ -39307,7 +39295,7 @@
         <v>133</v>
       </c>
       <c r="E2236" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2237" spans="1:5">
@@ -39375,7 +39363,7 @@
         <v>134</v>
       </c>
       <c r="E2240" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="2241" spans="1:5">
@@ -39494,7 +39482,7 @@
         <v>130</v>
       </c>
       <c r="E2247" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2248" spans="1:5">
@@ -39511,7 +39499,7 @@
         <v>134</v>
       </c>
       <c r="E2248" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="2249" spans="1:5">
@@ -39596,7 +39584,7 @@
         <v>132</v>
       </c>
       <c r="E2253" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="2254" spans="1:5">
@@ -39732,7 +39720,7 @@
         <v>137</v>
       </c>
       <c r="E2261" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2262" spans="1:5">
@@ -39987,7 +39975,7 @@
         <v>130</v>
       </c>
       <c r="E2276" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2277" spans="1:5">
@@ -40191,7 +40179,7 @@
         <v>133</v>
       </c>
       <c r="E2288" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="2289" spans="1:5">
@@ -40242,7 +40230,7 @@
         <v>134</v>
       </c>
       <c r="E2291" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="2292" spans="1:5">
@@ -40310,7 +40298,7 @@
         <v>141</v>
       </c>
       <c r="E2295" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="2296" spans="1:5">
@@ -40344,7 +40332,7 @@
         <v>130</v>
       </c>
       <c r="E2297" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2298" spans="1:5">
@@ -40378,7 +40366,7 @@
         <v>133</v>
       </c>
       <c r="E2299" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="2300" spans="1:5">
@@ -40599,7 +40587,7 @@
         <v>130</v>
       </c>
       <c r="E2312" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2313" spans="1:5">
@@ -41092,7 +41080,7 @@
         <v>130</v>
       </c>
       <c r="E2341" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2342" spans="1:5">
@@ -41296,7 +41284,7 @@
         <v>133</v>
       </c>
       <c r="E2353" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="2354" spans="1:5">
@@ -41381,7 +41369,7 @@
         <v>134</v>
       </c>
       <c r="E2358" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2359" spans="1:5">
@@ -41466,7 +41454,7 @@
         <v>133</v>
       </c>
       <c r="E2363" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="2364" spans="1:5">
@@ -41483,7 +41471,7 @@
         <v>133</v>
       </c>
       <c r="E2364" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="2365" spans="1:5">
@@ -41704,7 +41692,7 @@
         <v>130</v>
       </c>
       <c r="E2377" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2378" spans="1:5">
@@ -41721,7 +41709,7 @@
         <v>134</v>
       </c>
       <c r="E2378" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="2379" spans="1:5">
@@ -41806,7 +41794,7 @@
         <v>132</v>
       </c>
       <c r="E2383" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="2384" spans="1:5">
@@ -41925,7 +41913,7 @@
         <v>137</v>
       </c>
       <c r="E2390" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="2391" spans="1:5">
@@ -42503,7 +42491,7 @@
         <v>134</v>
       </c>
       <c r="E2424" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="2425" spans="1:5">
@@ -42809,7 +42797,7 @@
         <v>130</v>
       </c>
       <c r="E2442" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2443" spans="1:5">
@@ -43608,7 +43596,7 @@
         <v>134</v>
       </c>
       <c r="E2489" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="2490" spans="1:5">
@@ -43676,7 +43664,7 @@
         <v>133</v>
       </c>
       <c r="E2493" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2494" spans="1:5">
@@ -44016,7 +44004,7 @@
         <v>132</v>
       </c>
       <c r="E2513" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="2514" spans="1:5">
@@ -44152,7 +44140,7 @@
         <v>137</v>
       </c>
       <c r="E2521" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2522" spans="1:5">
@@ -44254,7 +44242,7 @@
         <v>138</v>
       </c>
       <c r="E2527" t="s">
-        <v>230</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2528" spans="1:5">
@@ -44594,7 +44582,7 @@
         <v>139</v>
       </c>
       <c r="E2547" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2548" spans="1:5">
@@ -44662,7 +44650,7 @@
         <v>134</v>
       </c>
       <c r="E2551" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2552" spans="1:5">
@@ -44747,7 +44735,7 @@
         <v>130</v>
       </c>
       <c r="E2556" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="2557" spans="1:5">
@@ -44781,7 +44769,7 @@
         <v>134</v>
       </c>
       <c r="E2558" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="2559" spans="1:5">
@@ -44832,7 +44820,7 @@
         <v>134</v>
       </c>
       <c r="E2561" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="2562" spans="1:5">
@@ -44985,7 +44973,7 @@
         <v>134</v>
       </c>
       <c r="E2570" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="2571" spans="1:5">
@@ -45359,7 +45347,7 @@
         <v>143</v>
       </c>
       <c r="E2592" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="2593" spans="1:5">
@@ -45699,7 +45687,7 @@
         <v>139</v>
       </c>
       <c r="E2612" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2613" spans="1:5">
@@ -45767,7 +45755,7 @@
         <v>134</v>
       </c>
       <c r="E2616" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2617" spans="1:5">
@@ -45886,7 +45874,7 @@
         <v>130</v>
       </c>
       <c r="E2623" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="2624" spans="1:5">
@@ -45903,7 +45891,7 @@
         <v>133</v>
       </c>
       <c r="E2624" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2625" spans="1:5">
@@ -45971,7 +45959,7 @@
         <v>141</v>
       </c>
       <c r="E2628" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2629" spans="1:5">
@@ -46141,7 +46129,7 @@
         <v>134</v>
       </c>
       <c r="E2638" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="2639" spans="1:5">
@@ -46600,7 +46588,7 @@
         <v>133</v>
       </c>
       <c r="E2665" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="2666" spans="1:5">
@@ -46617,7 +46605,7 @@
         <v>130</v>
       </c>
       <c r="E2666" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2667" spans="1:5">
@@ -46804,7 +46792,7 @@
         <v>139</v>
       </c>
       <c r="E2677" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2678" spans="1:5">
@@ -46872,7 +46860,7 @@
         <v>134</v>
       </c>
       <c r="E2681" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2682" spans="1:5">
@@ -46923,7 +46911,7 @@
         <v>134</v>
       </c>
       <c r="E2684" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="2685" spans="1:5">
@@ -46991,7 +46979,7 @@
         <v>134</v>
       </c>
       <c r="E2688" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="2689" spans="1:5">
@@ -47195,7 +47183,7 @@
         <v>133</v>
       </c>
       <c r="E2700" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="2701" spans="1:5">
@@ -47246,7 +47234,7 @@
         <v>134</v>
       </c>
       <c r="E2703" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="2704" spans="1:5">
@@ -47382,7 +47370,7 @@
         <v>134</v>
       </c>
       <c r="E2711" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2712" spans="1:5">
@@ -47467,7 +47455,7 @@
         <v>137</v>
       </c>
       <c r="E2716" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2717" spans="1:5">
@@ -47569,7 +47557,7 @@
         <v>143</v>
       </c>
       <c r="E2722" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="2723" spans="1:5">
@@ -47909,7 +47897,7 @@
         <v>139</v>
       </c>
       <c r="E2742" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2743" spans="1:5">
@@ -47977,7 +47965,7 @@
         <v>134</v>
       </c>
       <c r="E2746" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2747" spans="1:5">
@@ -48062,7 +48050,7 @@
         <v>134</v>
       </c>
       <c r="E2751" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="2752" spans="1:5">
@@ -48334,7 +48322,7 @@
         <v>130</v>
       </c>
       <c r="E2767" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2768" spans="1:5">
@@ -48351,7 +48339,7 @@
         <v>134</v>
       </c>
       <c r="E2768" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="2769" spans="1:5">
@@ -48674,7 +48662,7 @@
         <v>143</v>
       </c>
       <c r="E2787" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="2788" spans="1:5">
@@ -48776,7 +48764,7 @@
         <v>134</v>
       </c>
       <c r="E2793" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="2794" spans="1:5">
@@ -49286,7 +49274,7 @@
         <v>147</v>
       </c>
       <c r="E2823" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2824" spans="1:5">
@@ -49456,7 +49444,7 @@
         <v>134</v>
       </c>
       <c r="E2833" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="2834" spans="1:5">
@@ -49626,7 +49614,7 @@
         <v>139</v>
       </c>
       <c r="E2843" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="2844" spans="1:5">
@@ -50323,7 +50311,7 @@
         <v>133</v>
       </c>
       <c r="E2884" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2885" spans="1:5">
@@ -50544,7 +50532,7 @@
         <v>130</v>
       </c>
       <c r="E2897" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2898" spans="1:5">
@@ -51020,7 +51008,7 @@
         <v>133</v>
       </c>
       <c r="E2925" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="2926" spans="1:5">
@@ -51326,7 +51314,7 @@
         <v>134</v>
       </c>
       <c r="E2943" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2944" spans="1:5">
@@ -51411,7 +51399,7 @@
         <v>133</v>
       </c>
       <c r="E2948" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2949" spans="1:5">
@@ -51428,7 +51416,7 @@
         <v>133</v>
       </c>
       <c r="E2949" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="2950" spans="1:5">
@@ -51887,7 +51875,7 @@
         <v>137</v>
       </c>
       <c r="E2976" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2977" spans="1:5">
@@ -52431,7 +52419,7 @@
         <v>134</v>
       </c>
       <c r="E3008" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="3009" spans="1:5">
@@ -52533,7 +52521,7 @@
         <v>133</v>
       </c>
       <c r="E3014" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="3015" spans="1:5">
@@ -52754,7 +52742,7 @@
         <v>130</v>
       </c>
       <c r="E3027" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3028" spans="1:5">
@@ -52771,7 +52759,7 @@
         <v>134</v>
       </c>
       <c r="E3028" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3029" spans="1:5">
@@ -53434,7 +53422,7 @@
         <v>139</v>
       </c>
       <c r="E3067" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3068" spans="1:5">
@@ -53553,7 +53541,7 @@
         <v>133</v>
       </c>
       <c r="E3074" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3075" spans="1:5">
@@ -53859,7 +53847,7 @@
         <v>130</v>
       </c>
       <c r="E3092" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3093" spans="1:5">
@@ -53876,7 +53864,7 @@
         <v>134</v>
       </c>
       <c r="E3093" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3094" spans="1:5">
@@ -54335,7 +54323,7 @@
         <v>133</v>
       </c>
       <c r="E3120" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3121" spans="1:5">
@@ -54675,7 +54663,7 @@
         <v>134</v>
       </c>
       <c r="E3140" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="3141" spans="1:5">
@@ -54692,7 +54680,7 @@
         <v>134</v>
       </c>
       <c r="E3141" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="3142" spans="1:5">
@@ -54709,7 +54697,7 @@
         <v>130</v>
       </c>
       <c r="E3142" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="3143" spans="1:5">
@@ -54927,10 +54915,10 @@
         <v>88</v>
       </c>
       <c r="D3155" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E3155" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3156" spans="1:5">
@@ -55117,7 +55105,7 @@
         <v>134</v>
       </c>
       <c r="E3166" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="3167" spans="1:5">
@@ -55202,7 +55190,7 @@
         <v>144</v>
       </c>
       <c r="E3171" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3172" spans="1:5">
@@ -55304,7 +55292,7 @@
         <v>143</v>
       </c>
       <c r="E3177" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3178" spans="1:5">
@@ -55406,7 +55394,7 @@
         <v>134</v>
       </c>
       <c r="E3183" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="3184" spans="1:5">
@@ -55661,7 +55649,7 @@
         <v>133</v>
       </c>
       <c r="E3198" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="3199" spans="1:5">
@@ -56307,7 +56295,7 @@
         <v>137</v>
       </c>
       <c r="E3236" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3237" spans="1:5">
@@ -56562,7 +56550,7 @@
         <v>130</v>
       </c>
       <c r="E3251" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="3252" spans="1:5">
@@ -56936,7 +56924,7 @@
         <v>130</v>
       </c>
       <c r="E3273" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="3274" spans="1:5">
@@ -57412,7 +57400,7 @@
         <v>137</v>
       </c>
       <c r="E3301" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3302" spans="1:5">
@@ -57514,7 +57502,7 @@
         <v>138</v>
       </c>
       <c r="E3307" t="s">
-        <v>230</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3308" spans="1:5">
@@ -57684,7 +57672,7 @@
         <v>148</v>
       </c>
       <c r="E3317" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3318" spans="1:5">
@@ -57701,7 +57689,7 @@
         <v>148</v>
       </c>
       <c r="E3318" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3319" spans="1:5">
@@ -57718,7 +57706,7 @@
         <v>150</v>
       </c>
       <c r="E3319" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3320" spans="1:5">
@@ -57735,7 +57723,7 @@
         <v>148</v>
       </c>
       <c r="E3320" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3321" spans="1:5">
@@ -57752,7 +57740,7 @@
         <v>148</v>
       </c>
       <c r="E3321" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3322" spans="1:5">
@@ -57769,7 +57757,7 @@
         <v>148</v>
       </c>
       <c r="E3322" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3323" spans="1:5">
@@ -57786,7 +57774,7 @@
         <v>148</v>
       </c>
       <c r="E3323" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3324" spans="1:5">
@@ -57803,7 +57791,7 @@
         <v>148</v>
       </c>
       <c r="E3324" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3325" spans="1:5">
@@ -57820,7 +57808,7 @@
         <v>148</v>
       </c>
       <c r="E3325" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3326" spans="1:5">
@@ -57837,7 +57825,7 @@
         <v>148</v>
       </c>
       <c r="E3326" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3327" spans="1:5">
@@ -57854,7 +57842,7 @@
         <v>148</v>
       </c>
       <c r="E3327" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3328" spans="1:5">
@@ -57871,7 +57859,7 @@
         <v>148</v>
       </c>
       <c r="E3328" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3329" spans="1:5">
@@ -57888,7 +57876,7 @@
         <v>148</v>
       </c>
       <c r="E3329" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3330" spans="1:5">
@@ -57905,7 +57893,7 @@
         <v>148</v>
       </c>
       <c r="E3330" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3331" spans="1:5">
@@ -57922,7 +57910,7 @@
         <v>148</v>
       </c>
       <c r="E3331" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3332" spans="1:5">
@@ -57939,7 +57927,7 @@
         <v>148</v>
       </c>
       <c r="E3332" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3333" spans="1:5">
@@ -57956,7 +57944,7 @@
         <v>148</v>
       </c>
       <c r="E3333" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3334" spans="1:5">
@@ -57973,7 +57961,7 @@
         <v>148</v>
       </c>
       <c r="E3334" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3335" spans="1:5">
@@ -57990,7 +57978,7 @@
         <v>148</v>
       </c>
       <c r="E3335" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3336" spans="1:5">
@@ -58007,7 +57995,7 @@
         <v>148</v>
       </c>
       <c r="E3336" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3337" spans="1:5">
@@ -58024,7 +58012,7 @@
         <v>148</v>
       </c>
       <c r="E3337" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3338" spans="1:5">
@@ -58041,7 +58029,7 @@
         <v>148</v>
       </c>
       <c r="E3338" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3339" spans="1:5">
@@ -58058,7 +58046,7 @@
         <v>148</v>
       </c>
       <c r="E3339" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3340" spans="1:5">
@@ -58075,7 +58063,7 @@
         <v>148</v>
       </c>
       <c r="E3340" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3341" spans="1:5">
@@ -58092,7 +58080,7 @@
         <v>150</v>
       </c>
       <c r="E3341" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3342" spans="1:5">
@@ -58109,7 +58097,7 @@
         <v>148</v>
       </c>
       <c r="E3342" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3343" spans="1:5">
@@ -58126,7 +58114,7 @@
         <v>148</v>
       </c>
       <c r="E3343" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3344" spans="1:5">
@@ -58143,7 +58131,7 @@
         <v>148</v>
       </c>
       <c r="E3344" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3345" spans="1:5">
@@ -58160,7 +58148,7 @@
         <v>148</v>
       </c>
       <c r="E3345" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3346" spans="1:5">
@@ -58177,7 +58165,7 @@
         <v>148</v>
       </c>
       <c r="E3346" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3347" spans="1:5">
@@ -58194,7 +58182,7 @@
         <v>148</v>
       </c>
       <c r="E3347" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3348" spans="1:5">
@@ -58211,7 +58199,7 @@
         <v>148</v>
       </c>
       <c r="E3348" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3349" spans="1:5">
@@ -58228,7 +58216,7 @@
         <v>148</v>
       </c>
       <c r="E3349" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3350" spans="1:5">
@@ -58245,7 +58233,7 @@
         <v>148</v>
       </c>
       <c r="E3350" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3351" spans="1:5">
@@ -58262,7 +58250,7 @@
         <v>148</v>
       </c>
       <c r="E3351" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3352" spans="1:5">
@@ -58279,7 +58267,7 @@
         <v>150</v>
       </c>
       <c r="E3352" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3353" spans="1:5">
@@ -58296,7 +58284,7 @@
         <v>148</v>
       </c>
       <c r="E3353" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3354" spans="1:5">
@@ -58313,7 +58301,7 @@
         <v>148</v>
       </c>
       <c r="E3354" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3355" spans="1:5">
@@ -58330,7 +58318,7 @@
         <v>148</v>
       </c>
       <c r="E3355" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3356" spans="1:5">
@@ -58347,7 +58335,7 @@
         <v>148</v>
       </c>
       <c r="E3356" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3357" spans="1:5">
@@ -58364,7 +58352,7 @@
         <v>150</v>
       </c>
       <c r="E3357" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3358" spans="1:5">
@@ -58381,7 +58369,7 @@
         <v>148</v>
       </c>
       <c r="E3358" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3359" spans="1:5">
@@ -58398,7 +58386,7 @@
         <v>148</v>
       </c>
       <c r="E3359" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3360" spans="1:5">
@@ -58415,7 +58403,7 @@
         <v>148</v>
       </c>
       <c r="E3360" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3361" spans="1:5">
@@ -58432,7 +58420,7 @@
         <v>148</v>
       </c>
       <c r="E3361" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3362" spans="1:5">
@@ -58449,7 +58437,7 @@
         <v>148</v>
       </c>
       <c r="E3362" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3363" spans="1:5">
@@ -58466,7 +58454,7 @@
         <v>148</v>
       </c>
       <c r="E3363" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3364" spans="1:5">
@@ -58483,7 +58471,7 @@
         <v>148</v>
       </c>
       <c r="E3364" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3365" spans="1:5">
@@ -58500,7 +58488,7 @@
         <v>148</v>
       </c>
       <c r="E3365" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3366" spans="1:5">
@@ -58517,7 +58505,7 @@
         <v>148</v>
       </c>
       <c r="E3366" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3367" spans="1:5">
@@ -58534,7 +58522,7 @@
         <v>148</v>
       </c>
       <c r="E3367" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3368" spans="1:5">
@@ -58548,7 +58536,7 @@
         <v>121</v>
       </c>
       <c r="E3368" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3369" spans="1:5">
@@ -58562,7 +58550,7 @@
         <v>121</v>
       </c>
       <c r="E3369" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3370" spans="1:5">
@@ -58576,7 +58564,7 @@
         <v>121</v>
       </c>
       <c r="E3370" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="3371" spans="1:5">
@@ -58590,7 +58578,7 @@
         <v>121</v>
       </c>
       <c r="E3371" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="3372" spans="1:5">
@@ -58604,7 +58592,7 @@
         <v>121</v>
       </c>
       <c r="E3372" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3373" spans="1:5">
@@ -58618,7 +58606,7 @@
         <v>121</v>
       </c>
       <c r="E3373" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3374" spans="1:5">
@@ -58632,7 +58620,7 @@
         <v>121</v>
       </c>
       <c r="E3374" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3375" spans="1:5">
@@ -58646,7 +58634,7 @@
         <v>121</v>
       </c>
       <c r="E3375" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3376" spans="1:5">
@@ -58660,7 +58648,7 @@
         <v>121</v>
       </c>
       <c r="E3376" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3377" spans="1:5">
@@ -58674,7 +58662,7 @@
         <v>121</v>
       </c>
       <c r="E3377" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3378" spans="1:5">
@@ -58688,7 +58676,7 @@
         <v>121</v>
       </c>
       <c r="E3378" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3379" spans="1:5">
@@ -58702,7 +58690,7 @@
         <v>121</v>
       </c>
       <c r="E3379" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3380" spans="1:5">
@@ -58716,7 +58704,7 @@
         <v>121</v>
       </c>
       <c r="E3380" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3381" spans="1:5">
@@ -58730,7 +58718,7 @@
         <v>121</v>
       </c>
       <c r="E3381" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3382" spans="1:5">
@@ -58744,7 +58732,7 @@
         <v>121</v>
       </c>
       <c r="E3382" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="3383" spans="1:5">
@@ -58758,7 +58746,7 @@
         <v>121</v>
       </c>
       <c r="E3383" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3384" spans="1:5">
@@ -58772,7 +58760,7 @@
         <v>121</v>
       </c>
       <c r="E3384" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3385" spans="1:5">
@@ -58786,7 +58774,7 @@
         <v>121</v>
       </c>
       <c r="E3385" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3386" spans="1:5">
@@ -58800,7 +58788,7 @@
         <v>121</v>
       </c>
       <c r="E3386" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3387" spans="1:5">
@@ -58814,7 +58802,7 @@
         <v>121</v>
       </c>
       <c r="E3387" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3388" spans="1:5">
@@ -58828,7 +58816,7 @@
         <v>121</v>
       </c>
       <c r="E3388" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3389" spans="1:5">
@@ -58842,7 +58830,7 @@
         <v>121</v>
       </c>
       <c r="E3389" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3390" spans="1:5">
@@ -58856,7 +58844,7 @@
         <v>121</v>
       </c>
       <c r="E3390" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="3391" spans="1:5">
@@ -58870,7 +58858,7 @@
         <v>121</v>
       </c>
       <c r="E3391" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3392" spans="1:5">
@@ -58884,7 +58872,7 @@
         <v>121</v>
       </c>
       <c r="E3392" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3393" spans="1:5">
@@ -58898,7 +58886,7 @@
         <v>121</v>
       </c>
       <c r="E3393" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3394" spans="1:5">
@@ -58912,7 +58900,7 @@
         <v>121</v>
       </c>
       <c r="E3394" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3395" spans="1:5">
@@ -58926,7 +58914,7 @@
         <v>121</v>
       </c>
       <c r="E3395" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="3396" spans="1:5">
@@ -58940,7 +58928,7 @@
         <v>121</v>
       </c>
       <c r="E3396" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3397" spans="1:5">
@@ -58954,7 +58942,7 @@
         <v>121</v>
       </c>
       <c r="E3397" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="3398" spans="1:5">
@@ -58968,7 +58956,7 @@
         <v>121</v>
       </c>
       <c r="E3398" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="3399" spans="1:5">
@@ -58982,7 +58970,7 @@
         <v>121</v>
       </c>
       <c r="E3399" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="3400" spans="1:5">
@@ -58996,7 +58984,7 @@
         <v>121</v>
       </c>
       <c r="E3400" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3401" spans="1:5">
@@ -59010,7 +58998,7 @@
         <v>121</v>
       </c>
       <c r="E3401" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="3402" spans="1:5">
@@ -59024,7 +59012,7 @@
         <v>121</v>
       </c>
       <c r="E3402" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3403" spans="1:5">
@@ -59038,7 +59026,7 @@
         <v>121</v>
       </c>
       <c r="E3403" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="3404" spans="1:5">
@@ -59052,7 +59040,7 @@
         <v>121</v>
       </c>
       <c r="E3404" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3405" spans="1:5">
@@ -59066,7 +59054,7 @@
         <v>121</v>
       </c>
       <c r="E3405" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="3406" spans="1:5">
@@ -59080,7 +59068,7 @@
         <v>121</v>
       </c>
       <c r="E3406" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3407" spans="1:5">
@@ -59094,7 +59082,7 @@
         <v>121</v>
       </c>
       <c r="E3407" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="3408" spans="1:5">
@@ -59108,7 +59096,7 @@
         <v>121</v>
       </c>
       <c r="E3408" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3409" spans="1:5">
@@ -59122,7 +59110,7 @@
         <v>121</v>
       </c>
       <c r="E3409" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3410" spans="1:5">
@@ -59136,7 +59124,7 @@
         <v>121</v>
       </c>
       <c r="E3410" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3411" spans="1:5">
@@ -59150,7 +59138,7 @@
         <v>121</v>
       </c>
       <c r="E3411" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3412" spans="1:5">
@@ -59164,7 +59152,7 @@
         <v>121</v>
       </c>
       <c r="E3412" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3413" spans="1:5">
@@ -59178,7 +59166,7 @@
         <v>121</v>
       </c>
       <c r="E3413" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3414" spans="1:5">
@@ -59192,7 +59180,7 @@
         <v>121</v>
       </c>
       <c r="E3414" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="3415" spans="1:5">
@@ -59206,7 +59194,7 @@
         <v>121</v>
       </c>
       <c r="E3415" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="3416" spans="1:5">
@@ -59220,7 +59208,7 @@
         <v>121</v>
       </c>
       <c r="E3416" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="3417" spans="1:5">
@@ -59234,7 +59222,7 @@
         <v>121</v>
       </c>
       <c r="E3417" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="3418" spans="1:5">
@@ -59248,7 +59236,7 @@
         <v>121</v>
       </c>
       <c r="E3418" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="3419" spans="1:5">
@@ -59262,7 +59250,7 @@
         <v>122</v>
       </c>
       <c r="E3419" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="3420" spans="1:5">
@@ -59276,7 +59264,7 @@
         <v>122</v>
       </c>
       <c r="E3420" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="3421" spans="1:5">
@@ -59304,7 +59292,7 @@
         <v>122</v>
       </c>
       <c r="E3422" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="3423" spans="1:5">
@@ -59332,7 +59320,7 @@
         <v>122</v>
       </c>
       <c r="E3424" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="3425" spans="1:5">
@@ -59374,7 +59362,7 @@
         <v>122</v>
       </c>
       <c r="E3427" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3428" spans="1:5">
@@ -59458,7 +59446,7 @@
         <v>122</v>
       </c>
       <c r="E3433" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="3434" spans="1:5">
@@ -59486,7 +59474,7 @@
         <v>122</v>
       </c>
       <c r="E3435" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3436" spans="1:5">
@@ -59528,7 +59516,7 @@
         <v>122</v>
       </c>
       <c r="E3438" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="3439" spans="1:5">
@@ -59556,7 +59544,7 @@
         <v>122</v>
       </c>
       <c r="E3440" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="3441" spans="1:5">
@@ -59570,7 +59558,7 @@
         <v>122</v>
       </c>
       <c r="E3441" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="3442" spans="1:5">
@@ -59598,7 +59586,7 @@
         <v>122</v>
       </c>
       <c r="E3443" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="3444" spans="1:5">
@@ -59696,7 +59684,7 @@
         <v>122</v>
       </c>
       <c r="E3450" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="3451" spans="1:5">
@@ -59738,7 +59726,7 @@
         <v>122</v>
       </c>
       <c r="E3453" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3454" spans="1:5">
@@ -59808,7 +59796,7 @@
         <v>122</v>
       </c>
       <c r="E3458" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="3459" spans="1:5">
@@ -59850,7 +59838,7 @@
         <v>122</v>
       </c>
       <c r="E3461" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="3462" spans="1:5">
@@ -59864,7 +59852,7 @@
         <v>122</v>
       </c>
       <c r="E3462" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="3463" spans="1:5">
@@ -59878,7 +59866,7 @@
         <v>122</v>
       </c>
       <c r="E3463" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="3464" spans="1:5">
@@ -60284,7 +60272,7 @@
         <v>123</v>
       </c>
       <c r="E3492" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="3493" spans="1:5">
@@ -60354,7 +60342,7 @@
         <v>123</v>
       </c>
       <c r="E3497" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3498" spans="1:5">
@@ -60368,7 +60356,7 @@
         <v>123</v>
       </c>
       <c r="E3498" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="3499" spans="1:5">
@@ -60466,7 +60454,7 @@
         <v>123</v>
       </c>
       <c r="E3505" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="3506" spans="1:5">
@@ -60536,7 +60524,7 @@
         <v>123</v>
       </c>
       <c r="E3510" t="s">
-        <v>298</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3511" spans="1:5">
@@ -60690,7 +60678,7 @@
         <v>124</v>
       </c>
       <c r="E3521" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3522" spans="1:5">
@@ -60886,7 +60874,7 @@
         <v>124</v>
       </c>
       <c r="E3535" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3536" spans="1:5">
@@ -60914,7 +60902,7 @@
         <v>124</v>
       </c>
       <c r="E3537" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3538" spans="1:5">
@@ -60928,7 +60916,7 @@
         <v>124</v>
       </c>
       <c r="E3538" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3539" spans="1:5">
@@ -60956,7 +60944,7 @@
         <v>124</v>
       </c>
       <c r="E3540" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3541" spans="1:5">
@@ -61054,7 +61042,7 @@
         <v>124</v>
       </c>
       <c r="E3547" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3548" spans="1:5">
@@ -61096,7 +61084,7 @@
         <v>124</v>
       </c>
       <c r="E3550" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3551" spans="1:5">
@@ -61124,7 +61112,7 @@
         <v>124</v>
       </c>
       <c r="E3552" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3553" spans="1:5">
@@ -61138,7 +61126,7 @@
         <v>124</v>
       </c>
       <c r="E3553" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3554" spans="1:5">
@@ -61152,7 +61140,7 @@
         <v>124</v>
       </c>
       <c r="E3554" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3555" spans="1:5">
@@ -61194,7 +61182,7 @@
         <v>124</v>
       </c>
       <c r="E3557" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3558" spans="1:5">
@@ -61264,7 +61252,7 @@
         <v>124</v>
       </c>
       <c r="E3562" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3563" spans="1:5">
@@ -61292,7 +61280,7 @@
         <v>124</v>
       </c>
       <c r="E3564" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3565" spans="1:5">
@@ -61320,7 +61308,7 @@
         <v>124</v>
       </c>
       <c r="E3566" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3567" spans="1:5">
@@ -61376,7 +61364,7 @@
         <v>124</v>
       </c>
       <c r="E3570" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3571" spans="1:5">
@@ -61404,7 +61392,7 @@
         <v>125</v>
       </c>
       <c r="E3572" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3573" spans="1:5">
@@ -61432,7 +61420,7 @@
         <v>125</v>
       </c>
       <c r="E3574" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3575" spans="1:5">
@@ -61446,7 +61434,7 @@
         <v>125</v>
       </c>
       <c r="E3575" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3576" spans="1:5">
@@ -61460,7 +61448,7 @@
         <v>125</v>
       </c>
       <c r="E3576" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3577" spans="1:5">
@@ -61474,7 +61462,7 @@
         <v>125</v>
       </c>
       <c r="E3577" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3578" spans="1:5">
@@ -61544,7 +61532,7 @@
         <v>125</v>
       </c>
       <c r="E3582" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3583" spans="1:5">
@@ -61586,7 +61574,7 @@
         <v>125</v>
       </c>
       <c r="E3585" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3586" spans="1:5">
@@ -61614,7 +61602,7 @@
         <v>125</v>
       </c>
       <c r="E3587" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3588" spans="1:5">
@@ -61628,7 +61616,7 @@
         <v>125</v>
       </c>
       <c r="E3588" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3589" spans="1:5">
@@ -61656,7 +61644,7 @@
         <v>125</v>
       </c>
       <c r="E3590" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3591" spans="1:5">
@@ -61670,7 +61658,7 @@
         <v>125</v>
       </c>
       <c r="E3591" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3592" spans="1:5">
@@ -61712,7 +61700,7 @@
         <v>125</v>
       </c>
       <c r="E3594" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3595" spans="1:5">
@@ -61726,7 +61714,7 @@
         <v>125</v>
       </c>
       <c r="E3595" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3596" spans="1:5">
@@ -61740,7 +61728,7 @@
         <v>125</v>
       </c>
       <c r="E3596" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3597" spans="1:5">
@@ -61754,7 +61742,7 @@
         <v>125</v>
       </c>
       <c r="E3597" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3598" spans="1:5">
@@ -61824,7 +61812,7 @@
         <v>125</v>
       </c>
       <c r="E3602" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3603" spans="1:5">
@@ -61838,7 +61826,7 @@
         <v>125</v>
       </c>
       <c r="E3603" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3604" spans="1:5">
@@ -61852,7 +61840,7 @@
         <v>125</v>
       </c>
       <c r="E3604" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3605" spans="1:5">
@@ -61866,7 +61854,7 @@
         <v>125</v>
       </c>
       <c r="E3605" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3606" spans="1:5">
@@ -61880,7 +61868,7 @@
         <v>125</v>
       </c>
       <c r="E3606" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3607" spans="1:5">
@@ -61894,7 +61882,7 @@
         <v>125</v>
       </c>
       <c r="E3607" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3608" spans="1:5">
@@ -61936,7 +61924,7 @@
         <v>125</v>
       </c>
       <c r="E3610" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3611" spans="1:5">
@@ -61950,7 +61938,7 @@
         <v>125</v>
       </c>
       <c r="E3611" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3612" spans="1:5">
@@ -61964,7 +61952,7 @@
         <v>125</v>
       </c>
       <c r="E3612" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3613" spans="1:5">
@@ -62020,7 +62008,7 @@
         <v>125</v>
       </c>
       <c r="E3616" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3617" spans="1:5">
@@ -62062,7 +62050,7 @@
         <v>125</v>
       </c>
       <c r="E3619" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3620" spans="1:5">
@@ -62076,7 +62064,7 @@
         <v>125</v>
       </c>
       <c r="E3620" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3621" spans="1:5">
@@ -62090,7 +62078,7 @@
         <v>125</v>
       </c>
       <c r="E3621" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3622" spans="1:5">
@@ -62104,7 +62092,7 @@
         <v>125</v>
       </c>
       <c r="E3622" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3623" spans="1:5">
@@ -64195,7 +64183,7 @@
         <v>146</v>
       </c>
       <c r="E3745" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="3746" spans="1:5">
@@ -64331,7 +64319,7 @@
         <v>146</v>
       </c>
       <c r="E3753" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="3754" spans="1:5">
@@ -64733,7 +64721,7 @@
         <v>129</v>
       </c>
       <c r="E3777" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="3778" spans="1:5">
@@ -64789,7 +64777,7 @@
         <v>129</v>
       </c>
       <c r="E3781" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="3782" spans="1:5">
@@ -64803,7 +64791,7 @@
         <v>129</v>
       </c>
       <c r="E3782" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="3783" spans="1:5">
@@ -64817,7 +64805,7 @@
         <v>129</v>
       </c>
       <c r="E3783" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="3784" spans="1:5">
@@ -64845,7 +64833,7 @@
         <v>129</v>
       </c>
       <c r="E3785" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="3786" spans="1:5">
@@ -64859,7 +64847,7 @@
         <v>129</v>
       </c>
       <c r="E3786" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="3787" spans="1:5">
@@ -64943,7 +64931,7 @@
         <v>129</v>
       </c>
       <c r="E3792" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="3793" spans="1:5">
@@ -64985,7 +64973,7 @@
         <v>129</v>
       </c>
       <c r="E3795" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="3796" spans="1:5">
@@ -64999,7 +64987,7 @@
         <v>129</v>
       </c>
       <c r="E3796" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="3797" spans="1:5">
@@ -65013,7 +65001,7 @@
         <v>129</v>
       </c>
       <c r="E3797" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="3798" spans="1:5">
@@ -65027,7 +65015,7 @@
         <v>129</v>
       </c>
       <c r="E3798" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="3799" spans="1:5">
@@ -65041,7 +65029,7 @@
         <v>129</v>
       </c>
       <c r="E3799" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="3800" spans="1:5">
@@ -65055,7 +65043,7 @@
         <v>129</v>
       </c>
       <c r="E3800" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="3801" spans="1:5">
@@ -65125,7 +65113,7 @@
         <v>129</v>
       </c>
       <c r="E3805" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="3806" spans="1:5">
@@ -65195,7 +65183,7 @@
         <v>129</v>
       </c>
       <c r="E3810" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="3811" spans="1:5">
@@ -65293,7 +65281,7 @@
         <v>129</v>
       </c>
       <c r="E3817" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="3818" spans="1:5">
@@ -65307,7 +65295,7 @@
         <v>129</v>
       </c>
       <c r="E3818" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="3819" spans="1:5">
@@ -65349,7 +65337,7 @@
         <v>129</v>
       </c>
       <c r="E3821" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="3822" spans="1:5">
@@ -65405,7 +65393,7 @@
         <v>129</v>
       </c>
       <c r="E3825" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="3826" spans="1:5">

</xml_diff>

<commit_message>
Diagnostics.py werkt nu voor de nieuwe array.
</commit_message>
<xml_diff>
--- a/Output/Dataframes/complete.xlsx
+++ b/Output/Dataframes/complete.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14998" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14998" uniqueCount="303">
   <si>
     <t>sample_id</t>
   </si>
@@ -641,9 +641,6 @@
   </si>
   <si>
     <t>Kalyan-Kerala/Null</t>
-  </si>
-  <si>
-    <t>Present</t>
   </si>
   <si>
     <t>*A/*C</t>
@@ -5227,7 +5224,7 @@
         <v>141</v>
       </c>
       <c r="E232" t="s">
-        <v>209</v>
+        <v>171</v>
       </c>
     </row>
     <row r="233" spans="1:5">
@@ -5244,7 +5241,7 @@
         <v>134</v>
       </c>
       <c r="E233" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="234" spans="1:5">
@@ -5567,7 +5564,7 @@
         <v>143</v>
       </c>
       <c r="E252" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="253" spans="1:5">
@@ -5584,7 +5581,7 @@
         <v>139</v>
       </c>
       <c r="E253" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="254" spans="1:5">
@@ -6043,7 +6040,7 @@
         <v>133</v>
       </c>
       <c r="E280" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="281" spans="1:5">
@@ -6094,7 +6091,7 @@
         <v>133</v>
       </c>
       <c r="E283" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="284" spans="1:5">
@@ -6179,7 +6176,7 @@
         <v>134</v>
       </c>
       <c r="E288" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="289" spans="1:5">
@@ -6349,7 +6346,7 @@
         <v>134</v>
       </c>
       <c r="E298" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="299" spans="1:5">
@@ -6808,7 +6805,7 @@
         <v>134</v>
       </c>
       <c r="E325" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="326" spans="1:5">
@@ -7012,7 +7009,7 @@
         <v>139</v>
       </c>
       <c r="E337" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="338" spans="1:5">
@@ -7080,7 +7077,7 @@
         <v>134</v>
       </c>
       <c r="E341" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="342" spans="1:5">
@@ -7199,7 +7196,7 @@
         <v>133</v>
       </c>
       <c r="E348" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="349" spans="1:5">
@@ -7216,7 +7213,7 @@
         <v>133</v>
       </c>
       <c r="E349" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="350" spans="1:5">
@@ -7267,7 +7264,7 @@
         <v>145</v>
       </c>
       <c r="E352" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="353" spans="1:5">
@@ -7437,7 +7434,7 @@
         <v>130</v>
       </c>
       <c r="E362" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="363" spans="1:5">
@@ -7454,7 +7451,7 @@
         <v>134</v>
       </c>
       <c r="E363" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="364" spans="1:5">
@@ -7675,7 +7672,7 @@
         <v>144</v>
       </c>
       <c r="E376" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="377" spans="1:5">
@@ -7777,7 +7774,7 @@
         <v>141</v>
       </c>
       <c r="E382" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="383" spans="1:5">
@@ -8270,7 +8267,7 @@
         <v>130</v>
       </c>
       <c r="E411" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="412" spans="1:5">
@@ -8304,7 +8301,7 @@
         <v>133</v>
       </c>
       <c r="E413" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="414" spans="1:5">
@@ -8321,7 +8318,7 @@
         <v>133</v>
       </c>
       <c r="E414" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="415" spans="1:5">
@@ -8542,7 +8539,7 @@
         <v>130</v>
       </c>
       <c r="E427" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="428" spans="1:5">
@@ -8780,7 +8777,7 @@
         <v>137</v>
       </c>
       <c r="E441" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="442" spans="1:5">
@@ -8899,7 +8896,7 @@
         <v>139</v>
       </c>
       <c r="E448" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="449" spans="1:5">
@@ -9035,7 +9032,7 @@
         <v>130</v>
       </c>
       <c r="E456" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="457" spans="1:5">
@@ -9358,7 +9355,7 @@
         <v>133</v>
       </c>
       <c r="E475" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="476" spans="1:5">
@@ -9409,7 +9406,7 @@
         <v>134</v>
       </c>
       <c r="E478" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="479" spans="1:5">
@@ -9494,7 +9491,7 @@
         <v>134</v>
       </c>
       <c r="E483" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="484" spans="1:5">
@@ -9647,7 +9644,7 @@
         <v>130</v>
       </c>
       <c r="E492" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="493" spans="1:5">
@@ -9664,7 +9661,7 @@
         <v>134</v>
       </c>
       <c r="E493" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="494" spans="1:5">
@@ -9987,7 +9984,7 @@
         <v>143</v>
       </c>
       <c r="E512" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="513" spans="1:5">
@@ -10514,7 +10511,7 @@
         <v>134</v>
       </c>
       <c r="E543" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="544" spans="1:5">
@@ -10531,7 +10528,7 @@
         <v>133</v>
       </c>
       <c r="E544" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="545" spans="1:5">
@@ -10752,7 +10749,7 @@
         <v>130</v>
       </c>
       <c r="E557" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="558" spans="1:5">
@@ -10769,7 +10766,7 @@
         <v>134</v>
       </c>
       <c r="E558" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="559" spans="1:5">
@@ -10990,7 +10987,7 @@
         <v>137</v>
       </c>
       <c r="E571" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="572" spans="1:5">
@@ -11194,7 +11191,7 @@
         <v>134</v>
       </c>
       <c r="E583" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="584" spans="1:5">
@@ -11551,7 +11548,7 @@
         <v>134</v>
       </c>
       <c r="E604" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="605" spans="1:5">
@@ -11585,7 +11582,7 @@
         <v>134</v>
       </c>
       <c r="E606" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="607" spans="1:5">
@@ -11857,7 +11854,7 @@
         <v>130</v>
       </c>
       <c r="E622" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="623" spans="1:5">
@@ -11874,7 +11871,7 @@
         <v>134</v>
       </c>
       <c r="E623" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="624" spans="1:5">
@@ -12554,7 +12551,7 @@
         <v>133</v>
       </c>
       <c r="E663" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="664" spans="1:5">
@@ -12656,7 +12653,7 @@
         <v>134</v>
       </c>
       <c r="E669" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="670" spans="1:5">
@@ -12809,7 +12806,7 @@
         <v>147</v>
       </c>
       <c r="E678" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="679" spans="1:5">
@@ -12928,7 +12925,7 @@
         <v>133</v>
       </c>
       <c r="E685" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="686" spans="1:5">
@@ -13064,7 +13061,7 @@
         <v>132</v>
       </c>
       <c r="E693" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="694" spans="1:5">
@@ -13438,7 +13435,7 @@
         <v>133</v>
       </c>
       <c r="E715" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="716" spans="1:5">
@@ -13778,7 +13775,7 @@
         <v>134</v>
       </c>
       <c r="E735" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="736" spans="1:5">
@@ -13829,7 +13826,7 @@
         <v>134</v>
       </c>
       <c r="E738" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="739" spans="1:5">
@@ -14067,7 +14064,7 @@
         <v>130</v>
       </c>
       <c r="E752" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="753" spans="1:5">
@@ -14084,7 +14081,7 @@
         <v>134</v>
       </c>
       <c r="E753" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="754" spans="1:5">
@@ -14169,7 +14166,7 @@
         <v>132</v>
       </c>
       <c r="E758" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="759" spans="1:5">
@@ -14305,7 +14302,7 @@
         <v>137</v>
       </c>
       <c r="E766" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="767" spans="1:5">
@@ -14424,7 +14421,7 @@
         <v>148</v>
       </c>
       <c r="E773" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="774" spans="1:5">
@@ -14866,7 +14863,7 @@
         <v>133</v>
       </c>
       <c r="E799" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="800" spans="1:5">
@@ -15172,7 +15169,7 @@
         <v>130</v>
       </c>
       <c r="E817" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="818" spans="1:5">
@@ -15189,7 +15186,7 @@
         <v>134</v>
       </c>
       <c r="E818" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="819" spans="1:5">
@@ -15852,7 +15849,7 @@
         <v>139</v>
       </c>
       <c r="E857" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="858" spans="1:5">
@@ -15988,7 +15985,7 @@
         <v>133</v>
       </c>
       <c r="E865" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="866" spans="1:5">
@@ -16039,7 +16036,7 @@
         <v>133</v>
       </c>
       <c r="E868" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="869" spans="1:5">
@@ -16277,7 +16274,7 @@
         <v>130</v>
       </c>
       <c r="E882" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="883" spans="1:5">
@@ -16294,7 +16291,7 @@
         <v>134</v>
       </c>
       <c r="E883" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="884" spans="1:5">
@@ -16974,7 +16971,7 @@
         <v>133</v>
       </c>
       <c r="E923" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="924" spans="1:5">
@@ -17059,7 +17056,7 @@
         <v>134</v>
       </c>
       <c r="E928" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="929" spans="1:5">
@@ -17144,7 +17141,7 @@
         <v>134</v>
       </c>
       <c r="E933" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="934" spans="1:5">
@@ -17161,7 +17158,7 @@
         <v>133</v>
       </c>
       <c r="E934" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="935" spans="1:5">
@@ -17263,7 +17260,7 @@
         <v>134</v>
       </c>
       <c r="E940" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="941" spans="1:5">
@@ -17382,7 +17379,7 @@
         <v>130</v>
       </c>
       <c r="E947" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="948" spans="1:5">
@@ -17399,7 +17396,7 @@
         <v>134</v>
       </c>
       <c r="E948" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="949" spans="1:5">
@@ -17739,7 +17736,7 @@
         <v>139</v>
       </c>
       <c r="E968" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="969" spans="1:5">
@@ -18079,7 +18076,7 @@
         <v>133</v>
       </c>
       <c r="E988" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="989" spans="1:5">
@@ -18198,7 +18195,7 @@
         <v>134</v>
       </c>
       <c r="E995" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="996" spans="1:5">
@@ -18249,7 +18246,7 @@
         <v>133</v>
       </c>
       <c r="E998" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="999" spans="1:5">
@@ -18266,7 +18263,7 @@
         <v>133</v>
       </c>
       <c r="E999" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="1000" spans="1:5">
@@ -18504,7 +18501,7 @@
         <v>134</v>
       </c>
       <c r="E1013" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="1014" spans="1:5">
@@ -18589,7 +18586,7 @@
         <v>132</v>
       </c>
       <c r="E1018" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="1019" spans="1:5">
@@ -18725,7 +18722,7 @@
         <v>144</v>
       </c>
       <c r="E1026" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="1027" spans="1:5">
@@ -19184,7 +19181,7 @@
         <v>133</v>
       </c>
       <c r="E1053" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="1054" spans="1:5">
@@ -19269,7 +19266,7 @@
         <v>134</v>
       </c>
       <c r="E1058" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="1059" spans="1:5">
@@ -19439,7 +19436,7 @@
         <v>147</v>
       </c>
       <c r="E1068" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="1069" spans="1:5">
@@ -19609,7 +19606,7 @@
         <v>134</v>
       </c>
       <c r="E1078" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="1079" spans="1:5">
@@ -19830,7 +19827,7 @@
         <v>144</v>
       </c>
       <c r="E1091" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="1092" spans="1:5">
@@ -20697,7 +20694,7 @@
         <v>130</v>
       </c>
       <c r="E1142" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="1143" spans="1:5">
@@ -20714,7 +20711,7 @@
         <v>134</v>
       </c>
       <c r="E1143" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="1144" spans="1:5">
@@ -20799,7 +20796,7 @@
         <v>132</v>
       </c>
       <c r="E1148" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="1149" spans="1:5">
@@ -20935,7 +20932,7 @@
         <v>137</v>
       </c>
       <c r="E1156" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="1157" spans="1:5">
@@ -21037,7 +21034,7 @@
         <v>138</v>
       </c>
       <c r="E1162" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="1163" spans="1:5">
@@ -21496,7 +21493,7 @@
         <v>133</v>
       </c>
       <c r="E1189" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="1190" spans="1:5">
@@ -21564,7 +21561,7 @@
         <v>134</v>
       </c>
       <c r="E1193" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="1194" spans="1:5">
@@ -22618,7 +22615,7 @@
         <v>134</v>
       </c>
       <c r="E1255" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="1256" spans="1:5">
@@ -22652,7 +22649,7 @@
         <v>130</v>
       </c>
       <c r="E1257" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="1258" spans="1:5">
@@ -22669,7 +22666,7 @@
         <v>133</v>
       </c>
       <c r="E1258" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="1259" spans="1:5">
@@ -22754,7 +22751,7 @@
         <v>134</v>
       </c>
       <c r="E1263" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="1264" spans="1:5">
@@ -23145,7 +23142,7 @@
         <v>144</v>
       </c>
       <c r="E1286" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="1287" spans="1:5">
@@ -23723,7 +23720,7 @@
         <v>141</v>
       </c>
       <c r="E1320" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="1321" spans="1:5">
@@ -23774,7 +23771,7 @@
         <v>133</v>
       </c>
       <c r="E1323" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="1324" spans="1:5">
@@ -24012,7 +24009,7 @@
         <v>130</v>
       </c>
       <c r="E1337" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="1338" spans="1:5">
@@ -24029,7 +24026,7 @@
         <v>134</v>
       </c>
       <c r="E1338" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="1339" spans="1:5">
@@ -24114,7 +24111,7 @@
         <v>132</v>
       </c>
       <c r="E1343" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="1344" spans="1:5">
@@ -24369,7 +24366,7 @@
         <v>139</v>
       </c>
       <c r="E1358" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="1359" spans="1:5">
@@ -24794,7 +24791,7 @@
         <v>134</v>
       </c>
       <c r="E1383" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="1384" spans="1:5">
@@ -24896,7 +24893,7 @@
         <v>133</v>
       </c>
       <c r="E1389" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="1390" spans="1:5">
@@ -25865,7 +25862,7 @@
         <v>134</v>
       </c>
       <c r="E1446" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="1447" spans="1:5">
@@ -25950,7 +25947,7 @@
         <v>134</v>
       </c>
       <c r="E1451" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="1452" spans="1:5">
@@ -26001,7 +25998,7 @@
         <v>133</v>
       </c>
       <c r="E1454" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="1455" spans="1:5">
@@ -26052,7 +26049,7 @@
         <v>145</v>
       </c>
       <c r="E1457" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="1458" spans="1:5">
@@ -26239,7 +26236,7 @@
         <v>134</v>
       </c>
       <c r="E1468" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="1469" spans="1:5">
@@ -26443,7 +26440,7 @@
         <v>137</v>
       </c>
       <c r="E1480" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="1481" spans="1:5">
@@ -26562,7 +26559,7 @@
         <v>143</v>
       </c>
       <c r="E1487" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="1488" spans="1:5">
@@ -26579,7 +26576,7 @@
         <v>139</v>
       </c>
       <c r="E1488" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="1489" spans="1:5">
@@ -27021,7 +27018,7 @@
         <v>133</v>
       </c>
       <c r="E1514" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="1515" spans="1:5">
@@ -27089,7 +27086,7 @@
         <v>134</v>
       </c>
       <c r="E1518" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="1519" spans="1:5">
@@ -27344,7 +27341,7 @@
         <v>134</v>
       </c>
       <c r="E1533" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="1534" spans="1:5">
@@ -27667,7 +27664,7 @@
         <v>138</v>
       </c>
       <c r="E1552" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="1553" spans="1:5">
@@ -28075,7 +28072,7 @@
         <v>133</v>
       </c>
       <c r="E1576" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="1577" spans="1:5">
@@ -28126,7 +28123,7 @@
         <v>133</v>
       </c>
       <c r="E1579" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="1580" spans="1:5">
@@ -28211,7 +28208,7 @@
         <v>133</v>
       </c>
       <c r="E1584" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="1585" spans="1:5">
@@ -28245,7 +28242,7 @@
         <v>133</v>
       </c>
       <c r="E1586" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="1587" spans="1:5">
@@ -28432,7 +28429,7 @@
         <v>130</v>
       </c>
       <c r="E1597" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="1598" spans="1:5">
@@ -28772,7 +28769,7 @@
         <v>143</v>
       </c>
       <c r="E1617" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="1618" spans="1:5">
@@ -29299,7 +29296,7 @@
         <v>133</v>
       </c>
       <c r="E1648" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="1649" spans="1:5">
@@ -29367,7 +29364,7 @@
         <v>145</v>
       </c>
       <c r="E1652" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="1653" spans="1:5">
@@ -29537,7 +29534,7 @@
         <v>130</v>
       </c>
       <c r="E1662" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="1663" spans="1:5">
@@ -29775,7 +29772,7 @@
         <v>144</v>
       </c>
       <c r="E1676" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="1677" spans="1:5">
@@ -30030,7 +30027,7 @@
         <v>130</v>
       </c>
       <c r="E1691" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="1692" spans="1:5">
@@ -30353,7 +30350,7 @@
         <v>133</v>
       </c>
       <c r="E1710" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="1711" spans="1:5">
@@ -30404,7 +30401,7 @@
         <v>134</v>
       </c>
       <c r="E1713" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="1714" spans="1:5">
@@ -30659,7 +30656,7 @@
         <v>134</v>
       </c>
       <c r="E1728" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="1729" spans="1:5">
@@ -31509,7 +31506,7 @@
         <v>134</v>
       </c>
       <c r="E1778" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="1779" spans="1:5">
@@ -31747,7 +31744,7 @@
         <v>130</v>
       </c>
       <c r="E1792" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="1793" spans="1:5">
@@ -31985,7 +31982,7 @@
         <v>144</v>
       </c>
       <c r="E1806" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="1807" spans="1:5">
@@ -32087,7 +32084,7 @@
         <v>138</v>
       </c>
       <c r="E1812" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="1813" spans="1:5">
@@ -32546,7 +32543,7 @@
         <v>133</v>
       </c>
       <c r="E1839" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="1840" spans="1:5">
@@ -32852,7 +32849,7 @@
         <v>130</v>
       </c>
       <c r="E1857" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="1858" spans="1:5">
@@ -32954,7 +32951,7 @@
         <v>132</v>
       </c>
       <c r="E1863" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="1864" spans="1:5">
@@ -33974,7 +33971,7 @@
         <v>134</v>
       </c>
       <c r="E1923" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="1924" spans="1:5">
@@ -34297,7 +34294,7 @@
         <v>138</v>
       </c>
       <c r="E1942" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="1943" spans="1:5">
@@ -34314,7 +34311,7 @@
         <v>148</v>
       </c>
       <c r="E1943" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="1944" spans="1:5">
@@ -34773,7 +34770,7 @@
         <v>141</v>
       </c>
       <c r="E1970" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="1971" spans="1:5">
@@ -34807,7 +34804,7 @@
         <v>130</v>
       </c>
       <c r="E1972" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="1973" spans="1:5">
@@ -34824,7 +34821,7 @@
         <v>133</v>
       </c>
       <c r="E1973" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="1974" spans="1:5">
@@ -35062,7 +35059,7 @@
         <v>130</v>
       </c>
       <c r="E1987" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="1988" spans="1:5">
@@ -35538,7 +35535,7 @@
         <v>133</v>
       </c>
       <c r="E2015" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="2016" spans="1:5">
@@ -35555,7 +35552,7 @@
         <v>130</v>
       </c>
       <c r="E2016" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2017" spans="1:5">
@@ -35742,7 +35739,7 @@
         <v>139</v>
       </c>
       <c r="E2027" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2028" spans="1:5">
@@ -35810,7 +35807,7 @@
         <v>134</v>
       </c>
       <c r="E2031" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2032" spans="1:5">
@@ -35895,7 +35892,7 @@
         <v>134</v>
       </c>
       <c r="E2036" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2037" spans="1:5">
@@ -35929,7 +35926,7 @@
         <v>133</v>
       </c>
       <c r="E2038" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2039" spans="1:5">
@@ -36014,7 +36011,7 @@
         <v>134</v>
       </c>
       <c r="E2043" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2044" spans="1:5">
@@ -36048,7 +36045,7 @@
         <v>134</v>
       </c>
       <c r="E2045" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="2046" spans="1:5">
@@ -36184,7 +36181,7 @@
         <v>134</v>
       </c>
       <c r="E2053" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="2054" spans="1:5">
@@ -36507,7 +36504,7 @@
         <v>141</v>
       </c>
       <c r="E2072" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2073" spans="1:5">
@@ -36983,7 +36980,7 @@
         <v>134</v>
       </c>
       <c r="E2100" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="2101" spans="1:5">
@@ -37051,7 +37048,7 @@
         <v>133</v>
       </c>
       <c r="E2104" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="2105" spans="1:5">
@@ -37272,7 +37269,7 @@
         <v>130</v>
       </c>
       <c r="E2117" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2118" spans="1:5">
@@ -37765,7 +37762,7 @@
         <v>130</v>
       </c>
       <c r="E2146" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2147" spans="1:5">
@@ -37969,7 +37966,7 @@
         <v>133</v>
       </c>
       <c r="E2158" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="2159" spans="1:5">
@@ -38071,7 +38068,7 @@
         <v>133</v>
       </c>
       <c r="E2164" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="2165" spans="1:5">
@@ -38139,7 +38136,7 @@
         <v>133</v>
       </c>
       <c r="E2168" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2169" spans="1:5">
@@ -38615,7 +38612,7 @@
         <v>144</v>
       </c>
       <c r="E2196" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="2197" spans="1:5">
@@ -38734,7 +38731,7 @@
         <v>139</v>
       </c>
       <c r="E2203" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2204" spans="1:5">
@@ -39125,7 +39122,7 @@
         <v>134</v>
       </c>
       <c r="E2226" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="2227" spans="1:5">
@@ -39210,7 +39207,7 @@
         <v>134</v>
       </c>
       <c r="E2231" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="2232" spans="1:5">
@@ -39244,7 +39241,7 @@
         <v>134</v>
       </c>
       <c r="E2233" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="2234" spans="1:5">
@@ -39295,7 +39292,7 @@
         <v>133</v>
       </c>
       <c r="E2236" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="2237" spans="1:5">
@@ -39363,7 +39360,7 @@
         <v>134</v>
       </c>
       <c r="E2240" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="2241" spans="1:5">
@@ -39482,7 +39479,7 @@
         <v>130</v>
       </c>
       <c r="E2247" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2248" spans="1:5">
@@ -39499,7 +39496,7 @@
         <v>134</v>
       </c>
       <c r="E2248" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2249" spans="1:5">
@@ -39584,7 +39581,7 @@
         <v>132</v>
       </c>
       <c r="E2253" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="2254" spans="1:5">
@@ -39720,7 +39717,7 @@
         <v>137</v>
       </c>
       <c r="E2261" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2262" spans="1:5">
@@ -39822,7 +39819,7 @@
         <v>141</v>
       </c>
       <c r="E2267" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2268" spans="1:5">
@@ -39839,7 +39836,7 @@
         <v>139</v>
       </c>
       <c r="E2268" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2269" spans="1:5">
@@ -39975,7 +39972,7 @@
         <v>130</v>
       </c>
       <c r="E2276" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2277" spans="1:5">
@@ -40179,7 +40176,7 @@
         <v>133</v>
       </c>
       <c r="E2288" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="2289" spans="1:5">
@@ -40230,7 +40227,7 @@
         <v>134</v>
       </c>
       <c r="E2291" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2292" spans="1:5">
@@ -40298,7 +40295,7 @@
         <v>141</v>
       </c>
       <c r="E2295" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="2296" spans="1:5">
@@ -40332,7 +40329,7 @@
         <v>130</v>
       </c>
       <c r="E2297" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="2298" spans="1:5">
@@ -40366,7 +40363,7 @@
         <v>133</v>
       </c>
       <c r="E2299" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2300" spans="1:5">
@@ -40587,7 +40584,7 @@
         <v>130</v>
       </c>
       <c r="E2312" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2313" spans="1:5">
@@ -40604,7 +40601,7 @@
         <v>134</v>
       </c>
       <c r="E2313" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="2314" spans="1:5">
@@ -41063,7 +41060,7 @@
         <v>134</v>
       </c>
       <c r="E2340" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="2341" spans="1:5">
@@ -41080,7 +41077,7 @@
         <v>130</v>
       </c>
       <c r="E2341" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2342" spans="1:5">
@@ -41284,7 +41281,7 @@
         <v>133</v>
       </c>
       <c r="E2353" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="2354" spans="1:5">
@@ -41369,7 +41366,7 @@
         <v>134</v>
       </c>
       <c r="E2358" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="2359" spans="1:5">
@@ -41403,7 +41400,7 @@
         <v>133</v>
       </c>
       <c r="E2360" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="2361" spans="1:5">
@@ -41454,7 +41451,7 @@
         <v>133</v>
       </c>
       <c r="E2363" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2364" spans="1:5">
@@ -41471,7 +41468,7 @@
         <v>133</v>
       </c>
       <c r="E2364" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2365" spans="1:5">
@@ -41692,7 +41689,7 @@
         <v>130</v>
       </c>
       <c r="E2377" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2378" spans="1:5">
@@ -41709,7 +41706,7 @@
         <v>134</v>
       </c>
       <c r="E2378" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2379" spans="1:5">
@@ -41794,7 +41791,7 @@
         <v>132</v>
       </c>
       <c r="E2383" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="2384" spans="1:5">
@@ -41913,7 +41910,7 @@
         <v>137</v>
       </c>
       <c r="E2390" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="2391" spans="1:5">
@@ -42168,7 +42165,7 @@
         <v>134</v>
       </c>
       <c r="E2405" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="2406" spans="1:5">
@@ -42491,7 +42488,7 @@
         <v>134</v>
       </c>
       <c r="E2424" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="2425" spans="1:5">
@@ -42797,7 +42794,7 @@
         <v>130</v>
       </c>
       <c r="E2442" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2443" spans="1:5">
@@ -43596,7 +43593,7 @@
         <v>134</v>
       </c>
       <c r="E2489" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="2490" spans="1:5">
@@ -43664,7 +43661,7 @@
         <v>133</v>
       </c>
       <c r="E2493" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="2494" spans="1:5">
@@ -44004,7 +44001,7 @@
         <v>132</v>
       </c>
       <c r="E2513" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="2514" spans="1:5">
@@ -44140,7 +44137,7 @@
         <v>137</v>
       </c>
       <c r="E2521" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2522" spans="1:5">
@@ -44242,7 +44239,7 @@
         <v>138</v>
       </c>
       <c r="E2527" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2528" spans="1:5">
@@ -44582,7 +44579,7 @@
         <v>139</v>
       </c>
       <c r="E2547" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2548" spans="1:5">
@@ -44650,7 +44647,7 @@
         <v>134</v>
       </c>
       <c r="E2551" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2552" spans="1:5">
@@ -44735,7 +44732,7 @@
         <v>130</v>
       </c>
       <c r="E2556" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="2557" spans="1:5">
@@ -44769,7 +44766,7 @@
         <v>134</v>
       </c>
       <c r="E2558" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2559" spans="1:5">
@@ -44820,7 +44817,7 @@
         <v>134</v>
       </c>
       <c r="E2561" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="2562" spans="1:5">
@@ -44973,7 +44970,7 @@
         <v>134</v>
       </c>
       <c r="E2570" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="2571" spans="1:5">
@@ -45347,7 +45344,7 @@
         <v>143</v>
       </c>
       <c r="E2592" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="2593" spans="1:5">
@@ -45687,7 +45684,7 @@
         <v>139</v>
       </c>
       <c r="E2612" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2613" spans="1:5">
@@ -45755,7 +45752,7 @@
         <v>134</v>
       </c>
       <c r="E2616" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2617" spans="1:5">
@@ -45840,7 +45837,7 @@
         <v>134</v>
       </c>
       <c r="E2621" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2622" spans="1:5">
@@ -45874,7 +45871,7 @@
         <v>130</v>
       </c>
       <c r="E2623" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="2624" spans="1:5">
@@ -45891,7 +45888,7 @@
         <v>133</v>
       </c>
       <c r="E2624" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="2625" spans="1:5">
@@ -45959,7 +45956,7 @@
         <v>141</v>
       </c>
       <c r="E2628" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2629" spans="1:5">
@@ -46129,7 +46126,7 @@
         <v>134</v>
       </c>
       <c r="E2638" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2639" spans="1:5">
@@ -46452,7 +46449,7 @@
         <v>141</v>
       </c>
       <c r="E2657" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2658" spans="1:5">
@@ -46469,7 +46466,7 @@
         <v>139</v>
       </c>
       <c r="E2658" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2659" spans="1:5">
@@ -46588,7 +46585,7 @@
         <v>133</v>
       </c>
       <c r="E2665" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="2666" spans="1:5">
@@ -46605,7 +46602,7 @@
         <v>130</v>
       </c>
       <c r="E2666" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2667" spans="1:5">
@@ -46792,7 +46789,7 @@
         <v>139</v>
       </c>
       <c r="E2677" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2678" spans="1:5">
@@ -46860,7 +46857,7 @@
         <v>134</v>
       </c>
       <c r="E2681" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2682" spans="1:5">
@@ -46911,7 +46908,7 @@
         <v>134</v>
       </c>
       <c r="E2684" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="2685" spans="1:5">
@@ -46979,7 +46976,7 @@
         <v>134</v>
       </c>
       <c r="E2688" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="2689" spans="1:5">
@@ -47180,10 +47177,10 @@
         <v>88</v>
       </c>
       <c r="D2700" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E2700" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="2701" spans="1:5">
@@ -47234,7 +47231,7 @@
         <v>134</v>
       </c>
       <c r="E2703" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="2704" spans="1:5">
@@ -47370,7 +47367,7 @@
         <v>134</v>
       </c>
       <c r="E2711" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="2712" spans="1:5">
@@ -47455,7 +47452,7 @@
         <v>137</v>
       </c>
       <c r="E2716" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2717" spans="1:5">
@@ -47557,7 +47554,7 @@
         <v>143</v>
       </c>
       <c r="E2722" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="2723" spans="1:5">
@@ -47574,7 +47571,7 @@
         <v>139</v>
       </c>
       <c r="E2723" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2724" spans="1:5">
@@ -47897,7 +47894,7 @@
         <v>139</v>
       </c>
       <c r="E2742" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2743" spans="1:5">
@@ -47965,7 +47962,7 @@
         <v>134</v>
       </c>
       <c r="E2746" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2747" spans="1:5">
@@ -48050,7 +48047,7 @@
         <v>134</v>
       </c>
       <c r="E2751" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2752" spans="1:5">
@@ -48322,7 +48319,7 @@
         <v>130</v>
       </c>
       <c r="E2767" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2768" spans="1:5">
@@ -48339,7 +48336,7 @@
         <v>134</v>
       </c>
       <c r="E2768" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2769" spans="1:5">
@@ -48662,7 +48659,7 @@
         <v>143</v>
       </c>
       <c r="E2787" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="2788" spans="1:5">
@@ -48764,7 +48761,7 @@
         <v>134</v>
       </c>
       <c r="E2793" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2794" spans="1:5">
@@ -49274,7 +49271,7 @@
         <v>147</v>
       </c>
       <c r="E2823" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="2824" spans="1:5">
@@ -49444,7 +49441,7 @@
         <v>134</v>
       </c>
       <c r="E2833" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2834" spans="1:5">
@@ -49614,7 +49611,7 @@
         <v>139</v>
       </c>
       <c r="E2843" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="2844" spans="1:5">
@@ -49784,7 +49781,7 @@
         <v>139</v>
       </c>
       <c r="E2853" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2854" spans="1:5">
@@ -50311,7 +50308,7 @@
         <v>133</v>
       </c>
       <c r="E2884" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="2885" spans="1:5">
@@ -50532,7 +50529,7 @@
         <v>130</v>
       </c>
       <c r="E2897" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2898" spans="1:5">
@@ -51008,7 +51005,7 @@
         <v>133</v>
       </c>
       <c r="E2925" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="2926" spans="1:5">
@@ -51314,7 +51311,7 @@
         <v>134</v>
       </c>
       <c r="E2943" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="2944" spans="1:5">
@@ -51399,7 +51396,7 @@
         <v>133</v>
       </c>
       <c r="E2948" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="2949" spans="1:5">
@@ -51416,7 +51413,7 @@
         <v>133</v>
       </c>
       <c r="E2949" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2950" spans="1:5">
@@ -51875,7 +51872,7 @@
         <v>137</v>
       </c>
       <c r="E2976" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2977" spans="1:5">
@@ -52419,7 +52416,7 @@
         <v>134</v>
       </c>
       <c r="E3008" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="3009" spans="1:5">
@@ -52521,7 +52518,7 @@
         <v>133</v>
       </c>
       <c r="E3014" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="3015" spans="1:5">
@@ -52589,7 +52586,7 @@
         <v>134</v>
       </c>
       <c r="E3018" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3019" spans="1:5">
@@ -52742,7 +52739,7 @@
         <v>130</v>
       </c>
       <c r="E3027" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3028" spans="1:5">
@@ -52759,7 +52756,7 @@
         <v>134</v>
       </c>
       <c r="E3028" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3029" spans="1:5">
@@ -53218,7 +53215,7 @@
         <v>134</v>
       </c>
       <c r="E3055" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3056" spans="1:5">
@@ -53422,7 +53419,7 @@
         <v>139</v>
       </c>
       <c r="E3067" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3068" spans="1:5">
@@ -53541,7 +53538,7 @@
         <v>133</v>
       </c>
       <c r="E3074" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3075" spans="1:5">
@@ -53677,7 +53674,7 @@
         <v>145</v>
       </c>
       <c r="E3082" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3083" spans="1:5">
@@ -53847,7 +53844,7 @@
         <v>130</v>
       </c>
       <c r="E3092" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3093" spans="1:5">
@@ -53864,7 +53861,7 @@
         <v>134</v>
       </c>
       <c r="E3093" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3094" spans="1:5">
@@ -54204,7 +54201,7 @@
         <v>139</v>
       </c>
       <c r="E3113" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3114" spans="1:5">
@@ -54323,7 +54320,7 @@
         <v>133</v>
       </c>
       <c r="E3120" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3121" spans="1:5">
@@ -54663,7 +54660,7 @@
         <v>134</v>
       </c>
       <c r="E3140" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="3141" spans="1:5">
@@ -54680,7 +54677,7 @@
         <v>134</v>
       </c>
       <c r="E3141" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="3142" spans="1:5">
@@ -54697,7 +54694,7 @@
         <v>130</v>
       </c>
       <c r="E3142" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3143" spans="1:5">
@@ -54918,7 +54915,7 @@
         <v>134</v>
       </c>
       <c r="E3155" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="3156" spans="1:5">
@@ -54969,7 +54966,7 @@
         <v>134</v>
       </c>
       <c r="E3158" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3159" spans="1:5">
@@ -55105,7 +55102,7 @@
         <v>134</v>
       </c>
       <c r="E3166" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="3167" spans="1:5">
@@ -55190,7 +55187,7 @@
         <v>144</v>
       </c>
       <c r="E3171" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3172" spans="1:5">
@@ -55292,7 +55289,7 @@
         <v>143</v>
       </c>
       <c r="E3177" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3178" spans="1:5">
@@ -55394,7 +55391,7 @@
         <v>134</v>
       </c>
       <c r="E3183" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="3184" spans="1:5">
@@ -55649,7 +55646,7 @@
         <v>133</v>
       </c>
       <c r="E3198" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3199" spans="1:5">
@@ -55785,7 +55782,7 @@
         <v>134</v>
       </c>
       <c r="E3206" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3207" spans="1:5">
@@ -56295,7 +56292,7 @@
         <v>137</v>
       </c>
       <c r="E3236" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3237" spans="1:5">
@@ -56550,7 +56547,7 @@
         <v>130</v>
       </c>
       <c r="E3251" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3252" spans="1:5">
@@ -56924,7 +56921,7 @@
         <v>130</v>
       </c>
       <c r="E3273" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="3274" spans="1:5">
@@ -57400,7 +57397,7 @@
         <v>137</v>
       </c>
       <c r="E3301" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3302" spans="1:5">
@@ -57502,7 +57499,7 @@
         <v>138</v>
       </c>
       <c r="E3307" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3308" spans="1:5">
@@ -57672,7 +57669,7 @@
         <v>148</v>
       </c>
       <c r="E3317" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3318" spans="1:5">
@@ -57689,7 +57686,7 @@
         <v>148</v>
       </c>
       <c r="E3318" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3319" spans="1:5">
@@ -57706,7 +57703,7 @@
         <v>150</v>
       </c>
       <c r="E3319" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="3320" spans="1:5">
@@ -57723,7 +57720,7 @@
         <v>148</v>
       </c>
       <c r="E3320" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3321" spans="1:5">
@@ -57740,7 +57737,7 @@
         <v>148</v>
       </c>
       <c r="E3321" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3322" spans="1:5">
@@ -57757,7 +57754,7 @@
         <v>148</v>
       </c>
       <c r="E3322" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3323" spans="1:5">
@@ -57774,7 +57771,7 @@
         <v>148</v>
       </c>
       <c r="E3323" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3324" spans="1:5">
@@ -57791,7 +57788,7 @@
         <v>148</v>
       </c>
       <c r="E3324" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3325" spans="1:5">
@@ -57808,7 +57805,7 @@
         <v>148</v>
       </c>
       <c r="E3325" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3326" spans="1:5">
@@ -57825,7 +57822,7 @@
         <v>148</v>
       </c>
       <c r="E3326" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3327" spans="1:5">
@@ -57842,7 +57839,7 @@
         <v>148</v>
       </c>
       <c r="E3327" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3328" spans="1:5">
@@ -57859,7 +57856,7 @@
         <v>148</v>
       </c>
       <c r="E3328" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3329" spans="1:5">
@@ -57876,7 +57873,7 @@
         <v>148</v>
       </c>
       <c r="E3329" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3330" spans="1:5">
@@ -57893,7 +57890,7 @@
         <v>148</v>
       </c>
       <c r="E3330" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3331" spans="1:5">
@@ -57910,7 +57907,7 @@
         <v>148</v>
       </c>
       <c r="E3331" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3332" spans="1:5">
@@ -57927,7 +57924,7 @@
         <v>148</v>
       </c>
       <c r="E3332" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3333" spans="1:5">
@@ -57944,7 +57941,7 @@
         <v>148</v>
       </c>
       <c r="E3333" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3334" spans="1:5">
@@ -57961,7 +57958,7 @@
         <v>148</v>
       </c>
       <c r="E3334" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3335" spans="1:5">
@@ -57978,7 +57975,7 @@
         <v>148</v>
       </c>
       <c r="E3335" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3336" spans="1:5">
@@ -57995,7 +57992,7 @@
         <v>148</v>
       </c>
       <c r="E3336" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3337" spans="1:5">
@@ -58012,7 +58009,7 @@
         <v>148</v>
       </c>
       <c r="E3337" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3338" spans="1:5">
@@ -58029,7 +58026,7 @@
         <v>148</v>
       </c>
       <c r="E3338" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3339" spans="1:5">
@@ -58046,7 +58043,7 @@
         <v>148</v>
       </c>
       <c r="E3339" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3340" spans="1:5">
@@ -58063,7 +58060,7 @@
         <v>148</v>
       </c>
       <c r="E3340" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3341" spans="1:5">
@@ -58080,7 +58077,7 @@
         <v>150</v>
       </c>
       <c r="E3341" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="3342" spans="1:5">
@@ -58097,7 +58094,7 @@
         <v>148</v>
       </c>
       <c r="E3342" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3343" spans="1:5">
@@ -58114,7 +58111,7 @@
         <v>148</v>
       </c>
       <c r="E3343" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3344" spans="1:5">
@@ -58131,7 +58128,7 @@
         <v>148</v>
       </c>
       <c r="E3344" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3345" spans="1:5">
@@ -58148,7 +58145,7 @@
         <v>148</v>
       </c>
       <c r="E3345" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3346" spans="1:5">
@@ -58165,7 +58162,7 @@
         <v>148</v>
       </c>
       <c r="E3346" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3347" spans="1:5">
@@ -58182,7 +58179,7 @@
         <v>148</v>
       </c>
       <c r="E3347" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3348" spans="1:5">
@@ -58199,7 +58196,7 @@
         <v>148</v>
       </c>
       <c r="E3348" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3349" spans="1:5">
@@ -58216,7 +58213,7 @@
         <v>148</v>
       </c>
       <c r="E3349" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3350" spans="1:5">
@@ -58233,7 +58230,7 @@
         <v>148</v>
       </c>
       <c r="E3350" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3351" spans="1:5">
@@ -58250,7 +58247,7 @@
         <v>148</v>
       </c>
       <c r="E3351" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3352" spans="1:5">
@@ -58267,7 +58264,7 @@
         <v>150</v>
       </c>
       <c r="E3352" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="3353" spans="1:5">
@@ -58284,7 +58281,7 @@
         <v>148</v>
       </c>
       <c r="E3353" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3354" spans="1:5">
@@ -58301,7 +58298,7 @@
         <v>148</v>
       </c>
       <c r="E3354" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3355" spans="1:5">
@@ -58318,7 +58315,7 @@
         <v>148</v>
       </c>
       <c r="E3355" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3356" spans="1:5">
@@ -58335,7 +58332,7 @@
         <v>148</v>
       </c>
       <c r="E3356" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3357" spans="1:5">
@@ -58352,7 +58349,7 @@
         <v>150</v>
       </c>
       <c r="E3357" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="3358" spans="1:5">
@@ -58369,7 +58366,7 @@
         <v>148</v>
       </c>
       <c r="E3358" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3359" spans="1:5">
@@ -58386,7 +58383,7 @@
         <v>148</v>
       </c>
       <c r="E3359" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3360" spans="1:5">
@@ -58403,7 +58400,7 @@
         <v>148</v>
       </c>
       <c r="E3360" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3361" spans="1:5">
@@ -58420,7 +58417,7 @@
         <v>148</v>
       </c>
       <c r="E3361" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3362" spans="1:5">
@@ -58437,7 +58434,7 @@
         <v>148</v>
       </c>
       <c r="E3362" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3363" spans="1:5">
@@ -58454,7 +58451,7 @@
         <v>148</v>
       </c>
       <c r="E3363" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3364" spans="1:5">
@@ -58471,7 +58468,7 @@
         <v>148</v>
       </c>
       <c r="E3364" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3365" spans="1:5">
@@ -58488,7 +58485,7 @@
         <v>148</v>
       </c>
       <c r="E3365" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3366" spans="1:5">
@@ -58505,7 +58502,7 @@
         <v>148</v>
       </c>
       <c r="E3366" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3367" spans="1:5">
@@ -58522,7 +58519,7 @@
         <v>148</v>
       </c>
       <c r="E3367" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3368" spans="1:5">
@@ -58536,7 +58533,7 @@
         <v>121</v>
       </c>
       <c r="E3368" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3369" spans="1:5">
@@ -58550,7 +58547,7 @@
         <v>121</v>
       </c>
       <c r="E3369" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3370" spans="1:5">
@@ -58564,7 +58561,7 @@
         <v>121</v>
       </c>
       <c r="E3370" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3371" spans="1:5">
@@ -58578,7 +58575,7 @@
         <v>121</v>
       </c>
       <c r="E3371" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3372" spans="1:5">
@@ -58592,7 +58589,7 @@
         <v>121</v>
       </c>
       <c r="E3372" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3373" spans="1:5">
@@ -58606,7 +58603,7 @@
         <v>121</v>
       </c>
       <c r="E3373" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3374" spans="1:5">
@@ -58620,7 +58617,7 @@
         <v>121</v>
       </c>
       <c r="E3374" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3375" spans="1:5">
@@ -58634,7 +58631,7 @@
         <v>121</v>
       </c>
       <c r="E3375" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3376" spans="1:5">
@@ -58648,7 +58645,7 @@
         <v>121</v>
       </c>
       <c r="E3376" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3377" spans="1:5">
@@ -58662,7 +58659,7 @@
         <v>121</v>
       </c>
       <c r="E3377" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3378" spans="1:5">
@@ -58676,7 +58673,7 @@
         <v>121</v>
       </c>
       <c r="E3378" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3379" spans="1:5">
@@ -58690,7 +58687,7 @@
         <v>121</v>
       </c>
       <c r="E3379" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3380" spans="1:5">
@@ -58704,7 +58701,7 @@
         <v>121</v>
       </c>
       <c r="E3380" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3381" spans="1:5">
@@ -58718,7 +58715,7 @@
         <v>121</v>
       </c>
       <c r="E3381" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3382" spans="1:5">
@@ -58732,7 +58729,7 @@
         <v>121</v>
       </c>
       <c r="E3382" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3383" spans="1:5">
@@ -58746,7 +58743,7 @@
         <v>121</v>
       </c>
       <c r="E3383" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3384" spans="1:5">
@@ -58760,7 +58757,7 @@
         <v>121</v>
       </c>
       <c r="E3384" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3385" spans="1:5">
@@ -58774,7 +58771,7 @@
         <v>121</v>
       </c>
       <c r="E3385" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3386" spans="1:5">
@@ -58788,7 +58785,7 @@
         <v>121</v>
       </c>
       <c r="E3386" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3387" spans="1:5">
@@ -58802,7 +58799,7 @@
         <v>121</v>
       </c>
       <c r="E3387" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3388" spans="1:5">
@@ -58816,7 +58813,7 @@
         <v>121</v>
       </c>
       <c r="E3388" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3389" spans="1:5">
@@ -58830,7 +58827,7 @@
         <v>121</v>
       </c>
       <c r="E3389" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3390" spans="1:5">
@@ -58844,7 +58841,7 @@
         <v>121</v>
       </c>
       <c r="E3390" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3391" spans="1:5">
@@ -58858,7 +58855,7 @@
         <v>121</v>
       </c>
       <c r="E3391" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3392" spans="1:5">
@@ -58872,7 +58869,7 @@
         <v>121</v>
       </c>
       <c r="E3392" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3393" spans="1:5">
@@ -58886,7 +58883,7 @@
         <v>121</v>
       </c>
       <c r="E3393" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3394" spans="1:5">
@@ -58900,7 +58897,7 @@
         <v>121</v>
       </c>
       <c r="E3394" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3395" spans="1:5">
@@ -58914,7 +58911,7 @@
         <v>121</v>
       </c>
       <c r="E3395" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3396" spans="1:5">
@@ -58928,7 +58925,7 @@
         <v>121</v>
       </c>
       <c r="E3396" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3397" spans="1:5">
@@ -58942,7 +58939,7 @@
         <v>121</v>
       </c>
       <c r="E3397" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3398" spans="1:5">
@@ -58956,7 +58953,7 @@
         <v>121</v>
       </c>
       <c r="E3398" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3399" spans="1:5">
@@ -58970,7 +58967,7 @@
         <v>121</v>
       </c>
       <c r="E3399" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="3400" spans="1:5">
@@ -58984,7 +58981,7 @@
         <v>121</v>
       </c>
       <c r="E3400" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3401" spans="1:5">
@@ -58998,7 +58995,7 @@
         <v>121</v>
       </c>
       <c r="E3401" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3402" spans="1:5">
@@ -59012,7 +59009,7 @@
         <v>121</v>
       </c>
       <c r="E3402" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3403" spans="1:5">
@@ -59026,7 +59023,7 @@
         <v>121</v>
       </c>
       <c r="E3403" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3404" spans="1:5">
@@ -59040,7 +59037,7 @@
         <v>121</v>
       </c>
       <c r="E3404" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3405" spans="1:5">
@@ -59054,7 +59051,7 @@
         <v>121</v>
       </c>
       <c r="E3405" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="3406" spans="1:5">
@@ -59068,7 +59065,7 @@
         <v>121</v>
       </c>
       <c r="E3406" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3407" spans="1:5">
@@ -59082,7 +59079,7 @@
         <v>121</v>
       </c>
       <c r="E3407" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3408" spans="1:5">
@@ -59096,7 +59093,7 @@
         <v>121</v>
       </c>
       <c r="E3408" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3409" spans="1:5">
@@ -59110,7 +59107,7 @@
         <v>121</v>
       </c>
       <c r="E3409" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3410" spans="1:5">
@@ -59124,7 +59121,7 @@
         <v>121</v>
       </c>
       <c r="E3410" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3411" spans="1:5">
@@ -59138,7 +59135,7 @@
         <v>121</v>
       </c>
       <c r="E3411" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3412" spans="1:5">
@@ -59152,7 +59149,7 @@
         <v>121</v>
       </c>
       <c r="E3412" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3413" spans="1:5">
@@ -59166,7 +59163,7 @@
         <v>121</v>
       </c>
       <c r="E3413" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="3414" spans="1:5">
@@ -59180,7 +59177,7 @@
         <v>121</v>
       </c>
       <c r="E3414" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3415" spans="1:5">
@@ -59194,7 +59191,7 @@
         <v>121</v>
       </c>
       <c r="E3415" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="3416" spans="1:5">
@@ -59208,7 +59205,7 @@
         <v>121</v>
       </c>
       <c r="E3416" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3417" spans="1:5">
@@ -59222,7 +59219,7 @@
         <v>121</v>
       </c>
       <c r="E3417" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="3418" spans="1:5">
@@ -59236,7 +59233,7 @@
         <v>121</v>
       </c>
       <c r="E3418" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="3419" spans="1:5">
@@ -59250,7 +59247,7 @@
         <v>122</v>
       </c>
       <c r="E3419" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3420" spans="1:5">
@@ -59264,7 +59261,7 @@
         <v>122</v>
       </c>
       <c r="E3420" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3421" spans="1:5">
@@ -59292,7 +59289,7 @@
         <v>122</v>
       </c>
       <c r="E3422" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="3423" spans="1:5">
@@ -59306,7 +59303,7 @@
         <v>122</v>
       </c>
       <c r="E3423" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3424" spans="1:5">
@@ -59320,7 +59317,7 @@
         <v>122</v>
       </c>
       <c r="E3424" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="3425" spans="1:5">
@@ -59334,7 +59331,7 @@
         <v>122</v>
       </c>
       <c r="E3425" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3426" spans="1:5">
@@ -59362,7 +59359,7 @@
         <v>122</v>
       </c>
       <c r="E3427" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="3428" spans="1:5">
@@ -59376,7 +59373,7 @@
         <v>122</v>
       </c>
       <c r="E3428" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3429" spans="1:5">
@@ -59432,7 +59429,7 @@
         <v>122</v>
       </c>
       <c r="E3432" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3433" spans="1:5">
@@ -59446,7 +59443,7 @@
         <v>122</v>
       </c>
       <c r="E3433" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3434" spans="1:5">
@@ -59474,7 +59471,7 @@
         <v>122</v>
       </c>
       <c r="E3435" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3436" spans="1:5">
@@ -59488,7 +59485,7 @@
         <v>122</v>
       </c>
       <c r="E3436" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3437" spans="1:5">
@@ -59502,7 +59499,7 @@
         <v>122</v>
       </c>
       <c r="E3437" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3438" spans="1:5">
@@ -59516,7 +59513,7 @@
         <v>122</v>
       </c>
       <c r="E3438" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3439" spans="1:5">
@@ -59530,7 +59527,7 @@
         <v>122</v>
       </c>
       <c r="E3439" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3440" spans="1:5">
@@ -59544,7 +59541,7 @@
         <v>122</v>
       </c>
       <c r="E3440" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3441" spans="1:5">
@@ -59558,7 +59555,7 @@
         <v>122</v>
       </c>
       <c r="E3441" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="3442" spans="1:5">
@@ -59586,7 +59583,7 @@
         <v>122</v>
       </c>
       <c r="E3443" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="3444" spans="1:5">
@@ -59600,7 +59597,7 @@
         <v>122</v>
       </c>
       <c r="E3444" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3445" spans="1:5">
@@ -59642,7 +59639,7 @@
         <v>122</v>
       </c>
       <c r="E3447" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3448" spans="1:5">
@@ -59656,7 +59653,7 @@
         <v>122</v>
       </c>
       <c r="E3448" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3449" spans="1:5">
@@ -59684,7 +59681,7 @@
         <v>122</v>
       </c>
       <c r="E3450" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="3451" spans="1:5">
@@ -59698,7 +59695,7 @@
         <v>122</v>
       </c>
       <c r="E3451" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3452" spans="1:5">
@@ -59726,7 +59723,7 @@
         <v>122</v>
       </c>
       <c r="E3453" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="3454" spans="1:5">
@@ -59768,7 +59765,7 @@
         <v>122</v>
       </c>
       <c r="E3456" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3457" spans="1:5">
@@ -59782,7 +59779,7 @@
         <v>122</v>
       </c>
       <c r="E3457" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3458" spans="1:5">
@@ -59796,7 +59793,7 @@
         <v>122</v>
       </c>
       <c r="E3458" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="3459" spans="1:5">
@@ -59824,7 +59821,7 @@
         <v>122</v>
       </c>
       <c r="E3460" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3461" spans="1:5">
@@ -59838,7 +59835,7 @@
         <v>122</v>
       </c>
       <c r="E3461" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="3462" spans="1:5">
@@ -59852,7 +59849,7 @@
         <v>122</v>
       </c>
       <c r="E3462" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="3463" spans="1:5">
@@ -59866,7 +59863,7 @@
         <v>122</v>
       </c>
       <c r="E3463" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3464" spans="1:5">
@@ -59880,7 +59877,7 @@
         <v>122</v>
       </c>
       <c r="E3464" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3465" spans="1:5">
@@ -59950,7 +59947,7 @@
         <v>122</v>
       </c>
       <c r="E3469" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3470" spans="1:5">
@@ -60006,7 +60003,7 @@
         <v>123</v>
       </c>
       <c r="E3473" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3474" spans="1:5">
@@ -60062,7 +60059,7 @@
         <v>123</v>
       </c>
       <c r="E3477" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3478" spans="1:5">
@@ -60118,7 +60115,7 @@
         <v>123</v>
       </c>
       <c r="E3481" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3482" spans="1:5">
@@ -60244,7 +60241,7 @@
         <v>123</v>
       </c>
       <c r="E3490" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3491" spans="1:5">
@@ -60258,7 +60255,7 @@
         <v>123</v>
       </c>
       <c r="E3491" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3492" spans="1:5">
@@ -60272,7 +60269,7 @@
         <v>123</v>
       </c>
       <c r="E3492" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="3493" spans="1:5">
@@ -60300,7 +60297,7 @@
         <v>123</v>
       </c>
       <c r="E3494" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3495" spans="1:5">
@@ -60342,7 +60339,7 @@
         <v>123</v>
       </c>
       <c r="E3497" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3498" spans="1:5">
@@ -60356,7 +60353,7 @@
         <v>123</v>
       </c>
       <c r="E3498" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3499" spans="1:5">
@@ -60412,7 +60409,7 @@
         <v>123</v>
       </c>
       <c r="E3502" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3503" spans="1:5">
@@ -60454,7 +60451,7 @@
         <v>123</v>
       </c>
       <c r="E3505" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3506" spans="1:5">
@@ -60678,7 +60675,7 @@
         <v>124</v>
       </c>
       <c r="E3521" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3522" spans="1:5">
@@ -60874,7 +60871,7 @@
         <v>124</v>
       </c>
       <c r="E3535" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3536" spans="1:5">
@@ -60902,7 +60899,7 @@
         <v>124</v>
       </c>
       <c r="E3537" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3538" spans="1:5">
@@ -60916,7 +60913,7 @@
         <v>124</v>
       </c>
       <c r="E3538" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3539" spans="1:5">
@@ -60944,7 +60941,7 @@
         <v>124</v>
       </c>
       <c r="E3540" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3541" spans="1:5">
@@ -61042,7 +61039,7 @@
         <v>124</v>
       </c>
       <c r="E3547" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3548" spans="1:5">
@@ -61084,7 +61081,7 @@
         <v>124</v>
       </c>
       <c r="E3550" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3551" spans="1:5">
@@ -61112,7 +61109,7 @@
         <v>124</v>
       </c>
       <c r="E3552" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3553" spans="1:5">
@@ -61126,7 +61123,7 @@
         <v>124</v>
       </c>
       <c r="E3553" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3554" spans="1:5">
@@ -61140,7 +61137,7 @@
         <v>124</v>
       </c>
       <c r="E3554" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3555" spans="1:5">
@@ -61182,7 +61179,7 @@
         <v>124</v>
       </c>
       <c r="E3557" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3558" spans="1:5">
@@ -61252,7 +61249,7 @@
         <v>124</v>
       </c>
       <c r="E3562" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3563" spans="1:5">
@@ -61280,7 +61277,7 @@
         <v>124</v>
       </c>
       <c r="E3564" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3565" spans="1:5">
@@ -61308,7 +61305,7 @@
         <v>124</v>
       </c>
       <c r="E3566" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3567" spans="1:5">
@@ -61364,7 +61361,7 @@
         <v>124</v>
       </c>
       <c r="E3570" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="3571" spans="1:5">
@@ -61392,7 +61389,7 @@
         <v>125</v>
       </c>
       <c r="E3572" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3573" spans="1:5">
@@ -61420,7 +61417,7 @@
         <v>125</v>
       </c>
       <c r="E3574" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3575" spans="1:5">
@@ -61434,7 +61431,7 @@
         <v>125</v>
       </c>
       <c r="E3575" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3576" spans="1:5">
@@ -61448,7 +61445,7 @@
         <v>125</v>
       </c>
       <c r="E3576" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3577" spans="1:5">
@@ -61462,7 +61459,7 @@
         <v>125</v>
       </c>
       <c r="E3577" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3578" spans="1:5">
@@ -61532,7 +61529,7 @@
         <v>125</v>
       </c>
       <c r="E3582" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3583" spans="1:5">
@@ -61574,7 +61571,7 @@
         <v>125</v>
       </c>
       <c r="E3585" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3586" spans="1:5">
@@ -61602,7 +61599,7 @@
         <v>125</v>
       </c>
       <c r="E3587" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3588" spans="1:5">
@@ -61616,7 +61613,7 @@
         <v>125</v>
       </c>
       <c r="E3588" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3589" spans="1:5">
@@ -61644,7 +61641,7 @@
         <v>125</v>
       </c>
       <c r="E3590" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3591" spans="1:5">
@@ -61658,7 +61655,7 @@
         <v>125</v>
       </c>
       <c r="E3591" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3592" spans="1:5">
@@ -61700,7 +61697,7 @@
         <v>125</v>
       </c>
       <c r="E3594" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3595" spans="1:5">
@@ -61714,7 +61711,7 @@
         <v>125</v>
       </c>
       <c r="E3595" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3596" spans="1:5">
@@ -61728,7 +61725,7 @@
         <v>125</v>
       </c>
       <c r="E3596" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3597" spans="1:5">
@@ -61742,7 +61739,7 @@
         <v>125</v>
       </c>
       <c r="E3597" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3598" spans="1:5">
@@ -61812,7 +61809,7 @@
         <v>125</v>
       </c>
       <c r="E3602" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3603" spans="1:5">
@@ -61826,7 +61823,7 @@
         <v>125</v>
       </c>
       <c r="E3603" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3604" spans="1:5">
@@ -61840,7 +61837,7 @@
         <v>125</v>
       </c>
       <c r="E3604" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3605" spans="1:5">
@@ -61854,7 +61851,7 @@
         <v>125</v>
       </c>
       <c r="E3605" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3606" spans="1:5">
@@ -61868,7 +61865,7 @@
         <v>125</v>
       </c>
       <c r="E3606" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3607" spans="1:5">
@@ -61882,7 +61879,7 @@
         <v>125</v>
       </c>
       <c r="E3607" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3608" spans="1:5">
@@ -61924,7 +61921,7 @@
         <v>125</v>
       </c>
       <c r="E3610" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3611" spans="1:5">
@@ -61938,7 +61935,7 @@
         <v>125</v>
       </c>
       <c r="E3611" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3612" spans="1:5">
@@ -61952,7 +61949,7 @@
         <v>125</v>
       </c>
       <c r="E3612" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3613" spans="1:5">
@@ -62008,7 +62005,7 @@
         <v>125</v>
       </c>
       <c r="E3616" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3617" spans="1:5">
@@ -62050,7 +62047,7 @@
         <v>125</v>
       </c>
       <c r="E3619" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3620" spans="1:5">
@@ -62064,7 +62061,7 @@
         <v>125</v>
       </c>
       <c r="E3620" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3621" spans="1:5">
@@ -62078,7 +62075,7 @@
         <v>125</v>
       </c>
       <c r="E3621" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3622" spans="1:5">
@@ -62092,7 +62089,7 @@
         <v>125</v>
       </c>
       <c r="E3622" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3623" spans="1:5">
@@ -64183,7 +64180,7 @@
         <v>146</v>
       </c>
       <c r="E3745" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3746" spans="1:5">
@@ -64319,7 +64316,7 @@
         <v>146</v>
       </c>
       <c r="E3753" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="3754" spans="1:5">
@@ -64721,7 +64718,7 @@
         <v>129</v>
       </c>
       <c r="E3777" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3778" spans="1:5">
@@ -64777,7 +64774,7 @@
         <v>129</v>
       </c>
       <c r="E3781" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="3782" spans="1:5">
@@ -64791,7 +64788,7 @@
         <v>129</v>
       </c>
       <c r="E3782" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="3783" spans="1:5">
@@ -64805,7 +64802,7 @@
         <v>129</v>
       </c>
       <c r="E3783" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="3784" spans="1:5">
@@ -64833,7 +64830,7 @@
         <v>129</v>
       </c>
       <c r="E3785" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="3786" spans="1:5">
@@ -64847,7 +64844,7 @@
         <v>129</v>
       </c>
       <c r="E3786" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="3787" spans="1:5">
@@ -64931,7 +64928,7 @@
         <v>129</v>
       </c>
       <c r="E3792" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="3793" spans="1:5">
@@ -64973,7 +64970,7 @@
         <v>129</v>
       </c>
       <c r="E3795" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3796" spans="1:5">
@@ -64987,7 +64984,7 @@
         <v>129</v>
       </c>
       <c r="E3796" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="3797" spans="1:5">
@@ -65001,7 +64998,7 @@
         <v>129</v>
       </c>
       <c r="E3797" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="3798" spans="1:5">
@@ -65015,7 +65012,7 @@
         <v>129</v>
       </c>
       <c r="E3798" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3799" spans="1:5">
@@ -65029,7 +65026,7 @@
         <v>129</v>
       </c>
       <c r="E3799" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="3800" spans="1:5">
@@ -65043,7 +65040,7 @@
         <v>129</v>
       </c>
       <c r="E3800" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="3801" spans="1:5">
@@ -65113,7 +65110,7 @@
         <v>129</v>
       </c>
       <c r="E3805" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="3806" spans="1:5">
@@ -65183,7 +65180,7 @@
         <v>129</v>
       </c>
       <c r="E3810" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="3811" spans="1:5">
@@ -65281,7 +65278,7 @@
         <v>129</v>
       </c>
       <c r="E3817" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="3818" spans="1:5">
@@ -65295,7 +65292,7 @@
         <v>129</v>
       </c>
       <c r="E3818" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3819" spans="1:5">
@@ -65337,7 +65334,7 @@
         <v>129</v>
       </c>
       <c r="E3821" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="3822" spans="1:5">
@@ -65393,7 +65390,7 @@
         <v>129</v>
       </c>
       <c r="E3825" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="3826" spans="1:5">

</xml_diff>